<commit_message>
Added upgrade names to the vehicle upgrades page
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\A2B-Project\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="156">
   <si>
     <t>Name</t>
   </si>
@@ -388,6 +388,111 @@
   </si>
   <si>
     <t>Price (millions)</t>
+  </si>
+  <si>
+    <t>Pirelli Race Tires</t>
+  </si>
+  <si>
+    <t>Michelin Race Tires</t>
+  </si>
+  <si>
+    <t>GoodYear Race Tires</t>
+  </si>
+  <si>
+    <t>Continental Race Tires</t>
+  </si>
+  <si>
+    <t>Bridestone Race Tires</t>
+  </si>
+  <si>
+    <t>Light Body Panels</t>
+  </si>
+  <si>
+    <t>Lightweight Engine</t>
+  </si>
+  <si>
+    <t>Weight Reduced Tires</t>
+  </si>
+  <si>
+    <t>Aluminum Chassis</t>
+  </si>
+  <si>
+    <t>Race Suspension</t>
+  </si>
+  <si>
+    <t>Street Suspension</t>
+  </si>
+  <si>
+    <t>Leaf Spring</t>
+  </si>
+  <si>
+    <t>Coil Spring</t>
+  </si>
+  <si>
+    <t>Torsion Beam Suspension</t>
+  </si>
+  <si>
+    <t>Short Stroke Engine</t>
+  </si>
+  <si>
+    <t>CarbonG6:G37 Car Frame</t>
+  </si>
+  <si>
+    <t>V8 Engine</t>
+  </si>
+  <si>
+    <t>V6 Engine</t>
+  </si>
+  <si>
+    <t>External Combustion Engine</t>
+  </si>
+  <si>
+    <t>Internal Combustion Engine</t>
+  </si>
+  <si>
+    <t>CTV Transmission</t>
+  </si>
+  <si>
+    <t>Manual Transmission</t>
+  </si>
+  <si>
+    <t>Semi-Automatic Transmission</t>
+  </si>
+  <si>
+    <t>Gear Selection Transmission</t>
+  </si>
+  <si>
+    <t>Reduced Frontal Pressure</t>
+  </si>
+  <si>
+    <t>Computer Generated Airflow</t>
+  </si>
+  <si>
+    <t>Reduced Turbulence</t>
+  </si>
+  <si>
+    <t>Bodywork Conversion</t>
+  </si>
+  <si>
+    <t>Rear Vacuum Reduction</t>
+  </si>
+  <si>
+    <t>Dual Airfoil Wing</t>
+  </si>
+  <si>
+    <t>Single Airfoil Wing</t>
+  </si>
+  <si>
+    <t>Retractable Spoiler</t>
+  </si>
+  <si>
+    <t>Carbon Fiber Spoiler</t>
+  </si>
+  <si>
+    <t>Frontal Wing Upgrade</t>
+  </si>
+  <si>
+    <t>Sequential manual transmission</t>
   </si>
 </sst>
 </file>
@@ -395,7 +500,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -430,7 +535,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -469,17 +574,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -570,11 +664,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -587,13 +753,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -602,19 +766,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2557,702 +2763,811 @@
   <dimension ref="B1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" customWidth="1"/>
-    <col min="4" max="5" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
     <col min="9" max="10" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="15" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="17">
         <v>6</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="10" t="s">
+      <c r="G3" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="18">
         <f>POWER(F3,1.15)</f>
         <v>7.8500773842522964</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="10" t="s">
+      <c r="G4" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="18">
         <f t="shared" ref="F5:F7" si="0">POWER(F4,1.15)</f>
         <v>10.693134479003202</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="10" t="s">
+      <c r="G5" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="18">
         <f t="shared" si="0"/>
         <v>15.257057498113838</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="10" t="s">
+      <c r="G6" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7"/>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="31"/>
+      <c r="C7" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="20">
         <f t="shared" si="0"/>
         <v>22.961031816314314</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="12" t="s">
+      <c r="G7" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="10" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="17">
         <v>5</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>145</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="24"/>
+      <c r="C9" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="18">
         <f>POWER(F8,1.17)</f>
         <v>6.5734733273769663</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="G9" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="I9" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="15" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="18">
         <f t="shared" ref="F10:F12" si="1">POWER(F9,1.17)</f>
         <v>9.0535736509971976</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="10" t="s">
+      <c r="G10" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" s="8" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="24"/>
+      <c r="C11" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="18">
         <f t="shared" si="1"/>
         <v>13.166775950563464</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="10" t="s">
+      <c r="G11" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="11" t="s">
+      <c r="K11" s="8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="20">
         <f t="shared" si="1"/>
         <v>20.407553856606096</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="10" t="s">
+      <c r="G12" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="17">
         <v>5</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="10" t="s">
+      <c r="G13" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="K13" s="11" t="s">
+      <c r="K13" s="8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="18">
         <f>POWER(F13,1.12)</f>
         <v>6.0652178558631524</v>
       </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="12" t="s">
+      <c r="G14" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="I14" s="12"/>
+      <c r="J14" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="K14" s="13" t="s">
+      <c r="K14" s="10" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="18">
         <f t="shared" ref="F15:F17" si="2">POWER(F14,1.12)</f>
         <v>7.529878583836755</v>
       </c>
+      <c r="G15" s="29" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="24"/>
+      <c r="C16" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="18">
         <f t="shared" si="2"/>
         <v>9.5940622111548404</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="4" t="s">
+      <c r="G16" s="29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="31"/>
+      <c r="C17" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="20">
         <f t="shared" si="2"/>
         <v>12.584699037675147</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="G17" s="30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="17">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="4" t="s">
+      <c r="G18" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="24"/>
+      <c r="C19" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="18">
         <f>POWER(F18,1.19)</f>
         <v>11.876188565032388</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="4" t="s">
+      <c r="G19" s="29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="24"/>
+      <c r="C20" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="18">
         <f t="shared" ref="F20:F22" si="3">POWER(F19,1.19)</f>
         <v>19.004906205455562</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="4" t="s">
+      <c r="G20" s="29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="24"/>
+      <c r="C21" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="18">
         <f t="shared" si="3"/>
         <v>33.254484458357737</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="4" t="s">
+      <c r="G21" s="29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="24"/>
+      <c r="C22" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="20">
         <f t="shared" si="3"/>
         <v>64.714523993093408</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="G22" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="17">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="4" t="s">
+      <c r="G23" s="32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="24"/>
+      <c r="C24" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="18">
         <f>POWER(F23,1.25)</f>
         <v>5.6568542494923806</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="4" t="s">
+      <c r="G24" s="33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="24"/>
+      <c r="C25" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="18">
         <f t="shared" ref="F25:F27" si="4">POWER(F24,1.25)</f>
         <v>8.7240618613220615</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="4" t="s">
+      <c r="G25" s="33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="24"/>
+      <c r="C26" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="18">
         <f t="shared" si="4"/>
         <v>14.993341072882401</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="7"/>
-      <c r="C27" s="4" t="s">
+      <c r="G26" s="33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="31"/>
+      <c r="C27" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F27" s="20">
         <f t="shared" si="4"/>
         <v>29.503465103338023</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="7" t="s">
+      <c r="G27" s="34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="17">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="4" t="s">
+      <c r="G28" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="24"/>
+      <c r="C29" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F29" s="18">
         <f>POWER(F28,1.1)</f>
         <v>12.58925411794168</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="4" t="s">
+      <c r="G29" s="33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="25"/>
+      <c r="C30" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="19">
+      <c r="F30" s="18">
         <f t="shared" ref="F30:F32" si="5">POWER(F29,1.1)</f>
         <v>16.218100973589316</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="4" t="s">
+      <c r="G30" s="33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="25"/>
+      <c r="C31" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="F31" s="19">
+      <c r="F31" s="18">
         <f t="shared" si="5"/>
         <v>21.428906011200613</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="4" t="s">
+      <c r="G31" s="33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="25"/>
+      <c r="C32" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F32" s="20">
         <f t="shared" si="5"/>
         <v>29.113874126187596</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="7" t="s">
+      <c r="G32" s="34" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="F33" s="19">
+      <c r="F33" s="17">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="4" t="s">
+      <c r="G33" s="32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="25"/>
+      <c r="C34" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F34" s="18">
         <f>POWER(F33,1.05)</f>
         <v>23.231726992830843</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-      <c r="C35" s="4" t="s">
+      <c r="G34" s="33" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="25"/>
+      <c r="C35" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="F35" s="19">
+      <c r="F35" s="18">
         <f t="shared" ref="F35:F37" si="6">POWER(F34,1.05)</f>
         <v>27.188520168752266</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-      <c r="C36" s="4" t="s">
+      <c r="G35" s="33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="25"/>
+      <c r="C36" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="F36" s="19">
+      <c r="F36" s="18">
         <f t="shared" si="6"/>
         <v>32.070434855082958</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="4" t="s">
+      <c r="G36" s="33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="26"/>
+      <c r="C37" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F37" s="20">
         <f t="shared" si="6"/>
         <v>38.142582228695794</v>
       </c>
+      <c r="G37" s="34" t="s">
+        <v>136</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G17" r:id="rId1" display="https://en.wikipedia.org/wiki/Sequential_manual_transmission"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added 5 race tracks to the game data
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -5,27 +5,27 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\A2B-Project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
-    <sheet name="Chart1" sheetId="4" r:id="rId2"/>
-    <sheet name="Blad2" sheetId="2" r:id="rId3"/>
-    <sheet name="Blad3" sheetId="3" r:id="rId4"/>
+    <sheet name="Drivers" sheetId="1" r:id="rId1"/>
+    <sheet name="Car Upgrades" sheetId="2" r:id="rId2"/>
+    <sheet name="Race Time Calculation" sheetId="3" r:id="rId3"/>
+    <sheet name="Chart1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$B$2:$H$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drivers!$B$2:$H$32</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="192">
   <si>
     <t>Name</t>
   </si>
@@ -493,6 +493,114 @@
   </si>
   <si>
     <t>Sequential manual transmission</t>
+  </si>
+  <si>
+    <t>Track Name</t>
+  </si>
+  <si>
+    <t>Amount of turns</t>
+  </si>
+  <si>
+    <t>Track total length</t>
+  </si>
+  <si>
+    <t>In Kilometers</t>
+  </si>
+  <si>
+    <t>Track max height difference</t>
+  </si>
+  <si>
+    <t>In Meters</t>
+  </si>
+  <si>
+    <t>Spa-Francorchamps, Belgium</t>
+  </si>
+  <si>
+    <t>Silverstone, United Kingdom</t>
+  </si>
+  <si>
+    <t>Monza, Italy</t>
+  </si>
+  <si>
+    <t>Longest straight track</t>
+  </si>
+  <si>
+    <t>Monte Carlo, Monaco</t>
+  </si>
+  <si>
+    <t>Independent of turn size</t>
+  </si>
+  <si>
+    <t>Baku City Circuit, Azerbaijan</t>
+  </si>
+  <si>
+    <t>20 Corners</t>
+  </si>
+  <si>
+    <t>6,003 km</t>
+  </si>
+  <si>
+    <t>26,8 m</t>
+  </si>
+  <si>
+    <t>2,2 km</t>
+  </si>
+  <si>
+    <t>7,004 km</t>
+  </si>
+  <si>
+    <t>102,2 m</t>
+  </si>
+  <si>
+    <t>2,4 km</t>
+  </si>
+  <si>
+    <t>18 Corners</t>
+  </si>
+  <si>
+    <t>5,891 km</t>
+  </si>
+  <si>
+    <t>11,3 m</t>
+  </si>
+  <si>
+    <t>1,0 km</t>
+  </si>
+  <si>
+    <t>11 Corners</t>
+  </si>
+  <si>
+    <t>5,793 km</t>
+  </si>
+  <si>
+    <t>12,8 m</t>
+  </si>
+  <si>
+    <t>1,1 km</t>
+  </si>
+  <si>
+    <t>42,0 m</t>
+  </si>
+  <si>
+    <t>3,337 km</t>
+  </si>
+  <si>
+    <t>19 Corners</t>
+  </si>
+  <si>
+    <t>0,7 km</t>
+  </si>
+  <si>
+    <t>Car's with better handling and acceleration have better performance on track's with more turns</t>
+  </si>
+  <si>
+    <t>Longer track lengths will cause longer racing times</t>
+  </si>
+  <si>
+    <t>Track's with better down force and more weight will have less problems with height difference</t>
+  </si>
+  <si>
+    <t>Track's with more speed will be faster on track's with longer straight tracks</t>
   </si>
 </sst>
 </file>
@@ -502,7 +610,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,6 +634,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -535,7 +658,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -736,11 +859,110 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -822,6 +1044,45 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2762,7 +3023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -3573,12 +3834,150 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="6" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="40"/>
+      <c r="C3" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="47" t="s">
+        <v>188</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added formula's to calculate race length, see Whats-App for important note
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\A2B-Project\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
   </bookViews>
@@ -20,12 +15,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drivers!$B$2:$H$32</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="208">
   <si>
     <t>Name</t>
   </si>
@@ -601,12 +596,65 @@
   </si>
   <si>
     <t>Track's with more speed will be faster on track's with longer straight tracks</t>
+  </si>
+  <si>
+    <t>Formula's</t>
+  </si>
+  <si>
+    <t>Laps</t>
+  </si>
+  <si>
+    <t>Standard amount</t>
+  </si>
+  <si>
+    <t>Randomizer = Random float between 0.8 and 1.2</t>
+  </si>
+  <si>
+    <t>Max Verstappen: 1h:40m:23s
+Adrian Sutil: 8h:21m:12s</t>
+  </si>
+  <si>
+    <t>Baku City Circuit Time = 130'000'000'000 * Laps * Randomizer * (Turns / ((Driver_Turning * Car_Handling ) * (Car_Acceleration * Driver_Acceleration) * (Car_Braking / Car_Weight))) * (Max_Height / (Car_Handling / Car_Weight)) * (Longest / (Car_Speed * Driver_Speed)) * (Length / (Car_Speed * Driver_Speed)</t>
+  </si>
+  <si>
+    <t>Spa-Francorchamps Time = 5'000'000'000 * Laps * Randomizer * (Turns / ((Driver_Turning * Car_Handling ) * (Car_Acceleration * Driver_Acceleration) * (Car_Braking / Car_Weight))) * (Max_Height / (Car_Handling / Car_Weight)) * (Longest / (Car_Speed * Driver_Speed)) * (Length / (Car_Speed * Driver_Speed)</t>
+  </si>
+  <si>
+    <t>Baku City Circuit Time = 25'000'000'000 * Laps * Randomizer * (Turns / ((Driver_Turning * Car_Handling ) * (Car_Acceleration * Driver_Acceleration) * (Car_Braking / Car_Weight))) * (Max_Height / (Car_Handling / Car_Weight)) * (Longest / (Car_Speed * Driver_Speed)) * (Length / (Car_Speed * Driver_Speed)</t>
+  </si>
+  <si>
+    <t>Note that worse driver stat's will dramatically extend the race length, so this will need to be fixed or something. Take in consideration that the formula we have right now is already complicated and I'm thankful that it even works :P Also note that I used the worst driver stats with best car stats, so worst driver + worst car will lead to even longer times</t>
+  </si>
+  <si>
+    <t>Approx time it'll take to finish the full race, without randomizer, both in most upgraded car's</t>
+  </si>
+  <si>
+    <t>Baku City Circuit Time = 131'000'000'000 * Laps * Randomizer * (Turns / ((Driver_Turning * Car_Handling ) * (Car_Acceleration * Driver_Acceleration) * (Car_Braking / Car_Weight))) * (Max_Height / (Car_Handling / Car_Weight)) * (Longest / (Car_Speed * Driver_Speed)) * (Length / (Car_Speed * Driver_Speed)</t>
+  </si>
+  <si>
+    <t>Max Verstappen: 1h:30m:05s
+Adrian Sutil: 7h:29m:49s</t>
+  </si>
+  <si>
+    <t>Max Verstappen: 1h:24m:04s
+Adrian Sutil: 6h:59m:46s</t>
+  </si>
+  <si>
+    <t>Max Verstappen: 1h:09m:17s
+Adrian Sutil: 5h:45m:56s</t>
+  </si>
+  <si>
+    <t>Baku City Circuit Time = 98'000'000'000 * Laps * Randomizer * (Turns / ((Driver_Turning * Car_Handling ) * (Car_Acceleration * Driver_Acceleration) * (Car_Braking / Car_Weight))) * (Max_Height / (Car_Handling / Car_Weight)) * (Longest / (Car_Speed * Driver_Speed)) * (Length / (Car_Speed * Driver_Speed)</t>
+  </si>
+  <si>
+    <t>Max Verstappen: 2h:38m:19s
+Adrian Sutil: 13h:11m:16s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -658,7 +706,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -880,32 +928,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -958,11 +984,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1054,39 +1130,67 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1102,9 +1206,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1116,6 +1220,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1141,7 +1246,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1162,11 +1267,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="393388584"/>
-        <c:axId val="393388256"/>
+        <c:axId val="136435968"/>
+        <c:axId val="136442240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="393388584"/>
+        <c:axId val="136435968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,10 +1310,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="393388256"/>
+        <c:crossAx val="136442240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1216,7 +1321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="393388256"/>
+        <c:axId val="136442240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,10 +1368,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="393388584"/>
+        <c:crossAx val="136435968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1304,7 +1409,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1857,7 +1962,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1868,13 +1973,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9291941" cy="6069654"/>
+    <xdr:ext cx="9310872" cy="6084186"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D42C97-3EA1-4707-94E5-704BAB9AF338}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{45D42C97-3EA1-4707-94E5-704BAB9AF338}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1898,9 +2003,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1938,9 +2043,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1973,26 +2078,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2025,26 +2113,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3834,147 +3905,228 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F10"/>
+  <dimension ref="B1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" customWidth="1"/>
+    <col min="9" max="9" width="82.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="41" t="s">
         <v>157</v>
       </c>
       <c r="D2" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="38" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="40"/>
-      <c r="C3" s="42" t="s">
+      <c r="G2" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="I2" s="44" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="39"/>
+      <c r="C3" s="40" t="s">
         <v>167</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="36" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="44" t="s">
+      <c r="G3" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="I3" s="45" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="50" t="s">
         <v>170</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="49" t="s">
         <v>171</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="50" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="G4" s="51">
+        <v>51</v>
+      </c>
+      <c r="I4" s="56" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="49" t="s">
         <v>169</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="50" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="44" t="s">
+      <c r="G5" s="51">
+        <v>44</v>
+      </c>
+      <c r="I5" s="58" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="49" t="s">
         <v>176</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="50" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="44" t="s">
+      <c r="G6" s="51">
+        <v>52</v>
+      </c>
+      <c r="I6" s="58" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="49" t="s">
         <v>180</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="50" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="45" t="s">
+      <c r="G7" s="51">
+        <v>53</v>
+      </c>
+      <c r="I7" s="58" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="54" t="s">
         <v>185</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="54" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="47" t="s">
+      <c r="G8" s="55">
+        <v>78</v>
+      </c>
+      <c r="I8" s="58" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="43" t="s">
         <v>190</v>
       </c>
-      <c r="F10" s="48" t="s">
+      <c r="F10" s="43" t="s">
         <v>191</v>
+      </c>
+      <c r="I10" s="57" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="44"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="44" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="44" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="44" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="44" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="44" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="44" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a java file in a new project that has the base of our race simulation results, try it out for yourself!
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="177">
   <si>
     <t>Name</t>
   </si>
@@ -529,63 +529,6 @@
     <t>Baku City Circuit, Azerbaijan</t>
   </si>
   <si>
-    <t>20 Corners</t>
-  </si>
-  <si>
-    <t>6,003 km</t>
-  </si>
-  <si>
-    <t>26,8 m</t>
-  </si>
-  <si>
-    <t>2,2 km</t>
-  </si>
-  <si>
-    <t>7,004 km</t>
-  </si>
-  <si>
-    <t>102,2 m</t>
-  </si>
-  <si>
-    <t>2,4 km</t>
-  </si>
-  <si>
-    <t>18 Corners</t>
-  </si>
-  <si>
-    <t>5,891 km</t>
-  </si>
-  <si>
-    <t>11,3 m</t>
-  </si>
-  <si>
-    <t>1,0 km</t>
-  </si>
-  <si>
-    <t>11 Corners</t>
-  </si>
-  <si>
-    <t>5,793 km</t>
-  </si>
-  <si>
-    <t>12,8 m</t>
-  </si>
-  <si>
-    <t>1,1 km</t>
-  </si>
-  <si>
-    <t>42,0 m</t>
-  </si>
-  <si>
-    <t>3,337 km</t>
-  </si>
-  <si>
-    <t>19 Corners</t>
-  </si>
-  <si>
-    <t>0,7 km</t>
-  </si>
-  <si>
     <t>Car's with better handling and acceleration have better performance on track's with more turns</t>
   </si>
   <si>
@@ -598,57 +541,16 @@
     <t>Track's with more speed will be faster on track's with longer straight tracks</t>
   </si>
   <si>
-    <t>Formula's</t>
-  </si>
-  <si>
     <t>Laps</t>
   </si>
   <si>
     <t>Standard amount</t>
   </si>
   <si>
-    <t>Randomizer = Random float between 0.8 and 1.2</t>
-  </si>
-  <si>
-    <t>Max Verstappen: 1h:40m:23s
-Adrian Sutil: 8h:21m:12s</t>
-  </si>
-  <si>
-    <t>Baku City Circuit Time = 130'000'000'000 * Laps * Randomizer * (Turns / ((Driver_Turning * Car_Handling ) * (Car_Acceleration * Driver_Acceleration) * (Car_Braking / Car_Weight))) * (Max_Height / (Car_Handling / Car_Weight)) * (Longest / (Car_Speed * Driver_Speed)) * (Length / (Car_Speed * Driver_Speed)</t>
-  </si>
-  <si>
-    <t>Spa-Francorchamps Time = 5'000'000'000 * Laps * Randomizer * (Turns / ((Driver_Turning * Car_Handling ) * (Car_Acceleration * Driver_Acceleration) * (Car_Braking / Car_Weight))) * (Max_Height / (Car_Handling / Car_Weight)) * (Longest / (Car_Speed * Driver_Speed)) * (Length / (Car_Speed * Driver_Speed)</t>
-  </si>
-  <si>
-    <t>Baku City Circuit Time = 25'000'000'000 * Laps * Randomizer * (Turns / ((Driver_Turning * Car_Handling ) * (Car_Acceleration * Driver_Acceleration) * (Car_Braking / Car_Weight))) * (Max_Height / (Car_Handling / Car_Weight)) * (Longest / (Car_Speed * Driver_Speed)) * (Length / (Car_Speed * Driver_Speed)</t>
-  </si>
-  <si>
-    <t>Note that worse driver stat's will dramatically extend the race length, so this will need to be fixed or something. Take in consideration that the formula we have right now is already complicated and I'm thankful that it even works :P Also note that I used the worst driver stats with best car stats, so worst driver + worst car will lead to even longer times</t>
-  </si>
-  <si>
-    <t>Approx time it'll take to finish the full race, without randomizer, both in most upgraded car's</t>
-  </si>
-  <si>
-    <t>Baku City Circuit Time = 131'000'000'000 * Laps * Randomizer * (Turns / ((Driver_Turning * Car_Handling ) * (Car_Acceleration * Driver_Acceleration) * (Car_Braking / Car_Weight))) * (Max_Height / (Car_Handling / Car_Weight)) * (Longest / (Car_Speed * Driver_Speed)) * (Length / (Car_Speed * Driver_Speed)</t>
-  </si>
-  <si>
-    <t>Max Verstappen: 1h:30m:05s
-Adrian Sutil: 7h:29m:49s</t>
-  </si>
-  <si>
-    <t>Max Verstappen: 1h:24m:04s
-Adrian Sutil: 6h:59m:46s</t>
-  </si>
-  <si>
-    <t>Max Verstappen: 1h:09m:17s
-Adrian Sutil: 5h:45m:56s</t>
-  </si>
-  <si>
-    <t>Baku City Circuit Time = 98'000'000'000 * Laps * Randomizer * (Turns / ((Driver_Turning * Car_Handling ) * (Car_Acceleration * Driver_Acceleration) * (Car_Braking / Car_Weight))) * (Max_Height / (Car_Handling / Car_Weight)) * (Longest / (Car_Speed * Driver_Speed)) * (Length / (Car_Speed * Driver_Speed)</t>
-  </si>
-  <si>
-    <t>Max Verstappen: 2h:38m:19s
-Adrian Sutil: 13h:11m:16s</t>
+    <t>In meters</t>
+  </si>
+  <si>
+    <t>Track difficulty = 500/(Total Length / Amount of Turns)+(Max height diff / 100)+(1 / Longest straight)                      Scale of 1 to 5</t>
   </si>
 </sst>
 </file>
@@ -1220,7 +1122,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1267,11 +1168,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="136435968"/>
-        <c:axId val="136442240"/>
+        <c:axId val="143898880"/>
+        <c:axId val="143904768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="136435968"/>
+        <c:axId val="143898880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,7 +1214,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136442240"/>
+        <c:crossAx val="143904768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1321,7 +1222,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="136442240"/>
+        <c:axId val="143904768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1371,7 +1272,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="136435968"/>
+        <c:crossAx val="143898880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1979,7 +1880,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{45D42C97-3EA1-4707-94E5-704BAB9AF338}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D42C97-3EA1-4707-94E5-704BAB9AF338}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2292,7 +2193,7 @@
   <dimension ref="B2:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2346,7 +2247,7 @@
         <v>96</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" ref="G3:G32" si="0">ROUND(AVERAGE(D3:F3),1)</f>
+        <f>ROUND(AVERAGE(D3:F3),1)</f>
         <v>96</v>
       </c>
       <c r="H3" s="4">
@@ -2371,7 +2272,7 @@
         <v>93</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G3:G32" si="0">ROUND(AVERAGE(D4:F4),1)</f>
         <v>95</v>
       </c>
       <c r="H4" s="4">
@@ -3908,15 +3809,14 @@
   <dimension ref="B1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="6" width="27.42578125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="4.28515625" customWidth="1"/>
-    <col min="9" max="9" width="82.42578125" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3937,11 +3837,9 @@
         <v>165</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>193</v>
-      </c>
-      <c r="I2" s="44" t="s">
-        <v>192</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="39"/>
@@ -3949,7 +3847,7 @@
         <v>167</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>161</v>
@@ -3958,176 +3856,185 @@
         <v>159</v>
       </c>
       <c r="G3" s="47" t="s">
-        <v>194</v>
-      </c>
-      <c r="I3" s="45" t="s">
-        <v>201</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="I3" s="45"/>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="49" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>170</v>
-      </c>
-      <c r="E4" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="F4" s="50" t="s">
-        <v>172</v>
+      <c r="C4" s="49">
+        <v>20</v>
+      </c>
+      <c r="D4" s="50">
+        <v>6003</v>
+      </c>
+      <c r="E4" s="49">
+        <v>26.8</v>
+      </c>
+      <c r="F4" s="50">
+        <v>2.2000000000000002</v>
       </c>
       <c r="G4" s="51">
         <v>51</v>
       </c>
-      <c r="I4" s="56" t="s">
-        <v>196</v>
-      </c>
+      <c r="I4" s="56"/>
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="49" t="s">
-        <v>169</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="E5" s="49" t="s">
-        <v>174</v>
-      </c>
-      <c r="F5" s="50" t="s">
-        <v>175</v>
+      <c r="C5" s="49">
+        <v>20</v>
+      </c>
+      <c r="D5" s="50">
+        <v>7004</v>
+      </c>
+      <c r="E5" s="49">
+        <v>102.2</v>
+      </c>
+      <c r="F5" s="50">
+        <v>2.4</v>
       </c>
       <c r="G5" s="51">
         <v>44</v>
       </c>
-      <c r="I5" s="58" t="s">
-        <v>204</v>
-      </c>
+      <c r="I5" s="58"/>
     </row>
     <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="48" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="49" t="s">
-        <v>176</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>177</v>
-      </c>
-      <c r="E6" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="F6" s="50" t="s">
-        <v>179</v>
+      <c r="C6" s="49">
+        <v>18</v>
+      </c>
+      <c r="D6" s="50">
+        <v>5891</v>
+      </c>
+      <c r="E6" s="49">
+        <v>11.3</v>
+      </c>
+      <c r="F6" s="50">
+        <v>1</v>
       </c>
       <c r="G6" s="51">
         <v>52</v>
       </c>
-      <c r="I6" s="58" t="s">
-        <v>203</v>
-      </c>
+      <c r="I6" s="58"/>
     </row>
     <row r="7" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="48" t="s">
         <v>164</v>
       </c>
-      <c r="C7" s="49" t="s">
-        <v>180</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>181</v>
-      </c>
-      <c r="E7" s="49" t="s">
-        <v>182</v>
-      </c>
-      <c r="F7" s="50" t="s">
-        <v>183</v>
+      <c r="C7" s="49">
+        <v>11</v>
+      </c>
+      <c r="D7" s="50">
+        <v>5793</v>
+      </c>
+      <c r="E7" s="49">
+        <v>12.8</v>
+      </c>
+      <c r="F7" s="50">
+        <v>1.1000000000000001</v>
       </c>
       <c r="G7" s="51">
         <v>53</v>
       </c>
-      <c r="I7" s="58" t="s">
-        <v>205</v>
-      </c>
+      <c r="I7" s="58"/>
     </row>
     <row r="8" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="C8" s="53" t="s">
-        <v>186</v>
-      </c>
-      <c r="D8" s="54" t="s">
-        <v>185</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>184</v>
-      </c>
-      <c r="F8" s="54" t="s">
-        <v>187</v>
+      <c r="C8" s="53">
+        <v>19</v>
+      </c>
+      <c r="D8" s="54">
+        <v>3337</v>
+      </c>
+      <c r="E8" s="53">
+        <v>42</v>
+      </c>
+      <c r="F8" s="54">
+        <v>0.7</v>
       </c>
       <c r="G8" s="55">
         <v>78</v>
       </c>
-      <c r="I8" s="58" t="s">
-        <v>207</v>
-      </c>
+      <c r="I8" s="58"/>
     </row>
     <row r="10" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="42" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="I10" s="57" t="s">
-        <v>200</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="I10" s="57"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="44"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="44" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="44" t="s">
-        <v>198</v>
+      <c r="B15" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15">
+        <f>ROUND((500*(C4/D4)+(E4/100)+(1/F4)),1)</f>
+        <v>2.4</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="44" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="44" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="44" t="s">
-        <v>195</v>
-      </c>
+      <c r="B16" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C19" si="0">ROUND((500*(C5/D5)+(E5/100)+(1/F5)),1)</f>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="50" t="s">
+        <v>163</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="50" t="s">
+        <v>164</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added randomization (as choice) and if randomization is selected by the user, sort the race results accordingly.
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\A2B-Project\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Drivers" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drivers!$B$2:$H$32</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -556,7 +561,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -1092,7 +1097,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1108,9 +1113,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1147,7 +1152,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1211,7 +1216,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="143904768"/>
@@ -1269,7 +1274,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="143898880"/>
@@ -1310,7 +1315,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1880,7 +1885,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D42C97-3EA1-4707-94E5-704BAB9AF338}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D42C97-3EA1-4707-94E5-704BAB9AF338}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1904,9 +1909,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1944,9 +1949,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1979,9 +1984,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2014,9 +2036,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2192,8 +2231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,11 +2311,11 @@
         <v>93</v>
       </c>
       <c r="G4" s="4">
-        <f t="shared" ref="G3:G32" si="0">ROUND(AVERAGE(D4:F4),1)</f>
+        <f>ROUND(AVERAGE(D4:F4),1)</f>
         <v>95</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4:H32" si="1">(ROUND((G4/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" ref="H4:H32" si="0">(ROUND((G4/1.5)*1200000*1.1,-5))/1000000</f>
         <v>83.6</v>
       </c>
     </row>
@@ -2297,11 +2336,11 @@
         <v>95</v>
       </c>
       <c r="G5" s="4">
+        <f t="shared" ref="G5:G32" si="1">ROUND(AVERAGE(D5:F5),1)</f>
+        <v>94.7</v>
+      </c>
+      <c r="H5" s="4">
         <f t="shared" si="0"/>
-        <v>94.7</v>
-      </c>
-      <c r="H5" s="4">
-        <f t="shared" si="1"/>
         <v>83.3</v>
       </c>
     </row>
@@ -2322,11 +2361,11 @@
         <v>94</v>
       </c>
       <c r="G6" s="4">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+      <c r="H6" s="4">
         <f t="shared" si="0"/>
-        <v>94</v>
-      </c>
-      <c r="H6" s="4">
-        <f t="shared" si="1"/>
         <v>82.7</v>
       </c>
     </row>
@@ -2347,11 +2386,11 @@
         <v>90</v>
       </c>
       <c r="G7" s="4">
+        <f t="shared" si="1"/>
+        <v>92.3</v>
+      </c>
+      <c r="H7" s="4">
         <f t="shared" si="0"/>
-        <v>92.3</v>
-      </c>
-      <c r="H7" s="4">
-        <f t="shared" si="1"/>
         <v>81.2</v>
       </c>
     </row>
@@ -2372,11 +2411,11 @@
         <v>90</v>
       </c>
       <c r="G8" s="4">
+        <f t="shared" si="1"/>
+        <v>90.7</v>
+      </c>
+      <c r="H8" s="4">
         <f t="shared" si="0"/>
-        <v>90.7</v>
-      </c>
-      <c r="H8" s="4">
-        <f t="shared" si="1"/>
         <v>79.8</v>
       </c>
     </row>
@@ -2397,11 +2436,11 @@
         <v>85</v>
       </c>
       <c r="G9" s="4">
+        <f t="shared" si="1"/>
+        <v>85.7</v>
+      </c>
+      <c r="H9" s="4">
         <f t="shared" si="0"/>
-        <v>85.7</v>
-      </c>
-      <c r="H9" s="4">
-        <f t="shared" si="1"/>
         <v>75.400000000000006</v>
       </c>
     </row>
@@ -2422,11 +2461,11 @@
         <v>82</v>
       </c>
       <c r="G10" s="4">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="H10" s="4">
         <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-      <c r="H10" s="4">
-        <f t="shared" si="1"/>
         <v>73.900000000000006</v>
       </c>
     </row>
@@ -2447,11 +2486,11 @@
         <v>83</v>
       </c>
       <c r="G11" s="4">
+        <f t="shared" si="1"/>
+        <v>82.3</v>
+      </c>
+      <c r="H11" s="4">
         <f t="shared" si="0"/>
-        <v>82.3</v>
-      </c>
-      <c r="H11" s="4">
-        <f t="shared" si="1"/>
         <v>72.400000000000006</v>
       </c>
     </row>
@@ -2472,11 +2511,11 @@
         <v>82</v>
       </c>
       <c r="G12" s="4">
+        <f t="shared" si="1"/>
+        <v>79.7</v>
+      </c>
+      <c r="H12" s="4">
         <f t="shared" si="0"/>
-        <v>79.7</v>
-      </c>
-      <c r="H12" s="4">
-        <f t="shared" si="1"/>
         <v>70.099999999999994</v>
       </c>
     </row>
@@ -2488,7 +2527,7 @@
         <v>55</v>
       </c>
       <c r="D13" s="4">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E13" s="4">
         <v>74</v>
@@ -2497,12 +2536,12 @@
         <v>82</v>
       </c>
       <c r="G13" s="4">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="H13" s="4">
         <f t="shared" si="0"/>
-        <v>78.7</v>
-      </c>
-      <c r="H13" s="4">
-        <f t="shared" si="1"/>
-        <v>69.3</v>
+        <v>69.5</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -2522,11 +2561,11 @@
         <v>78</v>
       </c>
       <c r="G14" s="4">
+        <f t="shared" si="1"/>
+        <v>78.7</v>
+      </c>
+      <c r="H14" s="4">
         <f t="shared" si="0"/>
-        <v>78.7</v>
-      </c>
-      <c r="H14" s="4">
-        <f t="shared" si="1"/>
         <v>69.3</v>
       </c>
     </row>
@@ -2541,18 +2580,18 @@
         <v>80</v>
       </c>
       <c r="E15" s="4">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F15" s="4">
         <v>75</v>
       </c>
       <c r="G15" s="4">
+        <f t="shared" si="1"/>
+        <v>77.7</v>
+      </c>
+      <c r="H15" s="4">
         <f t="shared" si="0"/>
-        <v>77.3</v>
-      </c>
-      <c r="H15" s="4">
-        <f t="shared" si="1"/>
-        <v>68</v>
+        <v>68.400000000000006</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -2566,18 +2605,18 @@
         <v>78</v>
       </c>
       <c r="E16" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F16" s="4">
         <v>80</v>
       </c>
       <c r="G16" s="4">
+        <f t="shared" si="1"/>
+        <v>77.3</v>
+      </c>
+      <c r="H16" s="4">
         <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-      <c r="H16" s="4">
-        <f t="shared" si="1"/>
-        <v>67.8</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -2597,11 +2636,11 @@
         <v>79</v>
       </c>
       <c r="G17" s="4">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+      <c r="H17" s="4">
         <f t="shared" si="0"/>
-        <v>77</v>
-      </c>
-      <c r="H17" s="4">
-        <f t="shared" si="1"/>
         <v>67.8</v>
       </c>
     </row>
@@ -2622,11 +2661,11 @@
         <v>75</v>
       </c>
       <c r="G18" s="4">
+        <f t="shared" si="1"/>
+        <v>76.7</v>
+      </c>
+      <c r="H18" s="4">
         <f t="shared" si="0"/>
-        <v>76.7</v>
-      </c>
-      <c r="H18" s="4">
-        <f t="shared" si="1"/>
         <v>67.5</v>
       </c>
     </row>
@@ -2638,7 +2677,7 @@
         <v>94</v>
       </c>
       <c r="D19" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E19" s="4">
         <v>78</v>
@@ -2647,12 +2686,12 @@
         <v>74</v>
       </c>
       <c r="G19" s="4">
+        <f t="shared" si="1"/>
+        <v>75.3</v>
+      </c>
+      <c r="H19" s="4">
         <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="H19" s="4">
-        <f t="shared" si="1"/>
-        <v>66</v>
+        <v>66.3</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -2672,11 +2711,11 @@
         <v>71</v>
       </c>
       <c r="G20" s="4">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="H20" s="4">
         <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="H20" s="4">
-        <f t="shared" si="1"/>
         <v>66</v>
       </c>
     </row>
@@ -2697,11 +2736,11 @@
         <v>74</v>
       </c>
       <c r="G21" s="4">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="H21" s="4">
         <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-      <c r="H21" s="4">
-        <f t="shared" si="1"/>
         <v>65.099999999999994</v>
       </c>
     </row>
@@ -2722,11 +2761,11 @@
         <v>71</v>
       </c>
       <c r="G22" s="4">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="H22" s="4">
         <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-      <c r="H22" s="4">
-        <f t="shared" si="1"/>
         <v>63.4</v>
       </c>
     </row>
@@ -2747,11 +2786,11 @@
         <v>72</v>
       </c>
       <c r="G23" s="4">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="H23" s="4">
         <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
-      <c r="H23" s="4">
-        <f t="shared" si="1"/>
         <v>62.5</v>
       </c>
     </row>
@@ -2772,11 +2811,11 @@
         <v>69</v>
       </c>
       <c r="G24" s="4">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="H24" s="4">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="H24" s="4">
-        <f t="shared" si="1"/>
         <v>61.6</v>
       </c>
     </row>
@@ -2797,11 +2836,11 @@
         <v>66</v>
       </c>
       <c r="G25" s="4">
+        <f t="shared" si="1"/>
+        <v>69.3</v>
+      </c>
+      <c r="H25" s="4">
         <f t="shared" si="0"/>
-        <v>69.3</v>
-      </c>
-      <c r="H25" s="4">
-        <f t="shared" si="1"/>
         <v>61</v>
       </c>
     </row>
@@ -2822,11 +2861,11 @@
         <v>65</v>
       </c>
       <c r="G26" s="4">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="H26" s="4">
         <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="H26" s="4">
-        <f t="shared" si="1"/>
         <v>59.8</v>
       </c>
     </row>
@@ -2847,11 +2886,11 @@
         <v>64</v>
       </c>
       <c r="G27" s="4">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+      <c r="H27" s="4">
         <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="H27" s="4">
-        <f t="shared" si="1"/>
         <v>59</v>
       </c>
     </row>
@@ -2872,11 +2911,11 @@
         <v>60</v>
       </c>
       <c r="G28" s="4">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="H28" s="4">
         <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="H28" s="4">
-        <f t="shared" si="1"/>
         <v>58.1</v>
       </c>
     </row>
@@ -2897,11 +2936,11 @@
         <v>63</v>
       </c>
       <c r="G29" s="4">
+        <f t="shared" si="1"/>
+        <v>65.7</v>
+      </c>
+      <c r="H29" s="4">
         <f t="shared" si="0"/>
-        <v>65.7</v>
-      </c>
-      <c r="H29" s="4">
-        <f t="shared" si="1"/>
         <v>57.8</v>
       </c>
     </row>
@@ -2922,11 +2961,11 @@
         <v>62</v>
       </c>
       <c r="G30" s="4">
+        <f t="shared" si="1"/>
+        <v>65.7</v>
+      </c>
+      <c r="H30" s="4">
         <f t="shared" si="0"/>
-        <v>65.7</v>
-      </c>
-      <c r="H30" s="4">
-        <f t="shared" si="1"/>
         <v>57.8</v>
       </c>
     </row>
@@ -2947,11 +2986,11 @@
         <v>61</v>
       </c>
       <c r="G31" s="4">
+        <f t="shared" si="1"/>
+        <v>65.7</v>
+      </c>
+      <c r="H31" s="4">
         <f t="shared" si="0"/>
-        <v>65.7</v>
-      </c>
-      <c r="H31" s="4">
-        <f t="shared" si="1"/>
         <v>57.8</v>
       </c>
     </row>
@@ -2972,11 +3011,11 @@
         <v>61</v>
       </c>
       <c r="G32" s="4">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="H32" s="4">
         <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="H32" s="4">
-        <f t="shared" si="1"/>
         <v>56.3</v>
       </c>
     </row>
@@ -3808,7 +3847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the driver stats since i've changed them a tad for the race simulation application
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="169">
   <si>
     <t>Name</t>
   </si>
@@ -91,30 +91,6 @@
   </si>
   <si>
     <t>Esteban Gutierrez</t>
-  </si>
-  <si>
-    <t>Pastor Maldonado</t>
-  </si>
-  <si>
-    <t>Will Stevens</t>
-  </si>
-  <si>
-    <t>Roberto Merhi</t>
-  </si>
-  <si>
-    <t>Alexander Rossi</t>
-  </si>
-  <si>
-    <t>Adrian Sutil</t>
-  </si>
-  <si>
-    <t>Jean-Eric Vergne</t>
-  </si>
-  <si>
-    <t>Jules Bianchi</t>
-  </si>
-  <si>
-    <t>Max Chilton</t>
   </si>
   <si>
     <t>Speed</t>
@@ -945,7 +921,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1095,6 +1071,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2232,7 +2209,7 @@
   <dimension ref="B2:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H32" sqref="B25:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2251,22 +2228,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -2621,7 +2598,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C17" s="5">
         <v>12</v>
@@ -2820,204 +2797,76 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="5">
-        <v>71</v>
-      </c>
-      <c r="D25" s="4">
-        <v>70</v>
-      </c>
-      <c r="E25" s="4">
-        <v>72</v>
-      </c>
-      <c r="F25" s="4">
-        <v>66</v>
-      </c>
-      <c r="G25" s="4">
-        <f t="shared" si="1"/>
-        <v>69.3</v>
-      </c>
-      <c r="H25" s="4">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
+      <c r="B25" s="59"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="5">
-        <v>24</v>
-      </c>
-      <c r="D26" s="4">
-        <v>72</v>
-      </c>
-      <c r="E26" s="4">
-        <v>67</v>
-      </c>
-      <c r="F26" s="4">
-        <v>65</v>
-      </c>
-      <c r="G26" s="4">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="H26" s="4">
-        <f t="shared" si="0"/>
-        <v>59.8</v>
-      </c>
+      <c r="B26" s="59"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="5">
-        <v>67</v>
-      </c>
-      <c r="D27" s="4">
-        <v>69</v>
-      </c>
-      <c r="E27" s="4">
-        <v>68</v>
-      </c>
-      <c r="F27" s="4">
-        <v>64</v>
-      </c>
-      <c r="G27" s="4">
-        <f t="shared" si="1"/>
-        <v>67</v>
-      </c>
-      <c r="H27" s="4">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
+      <c r="B27" s="59"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="5">
-        <v>66</v>
-      </c>
-      <c r="D28" s="4">
-        <v>68</v>
-      </c>
-      <c r="E28" s="4">
-        <v>70</v>
-      </c>
-      <c r="F28" s="4">
-        <v>60</v>
-      </c>
-      <c r="G28" s="4">
-        <f t="shared" si="1"/>
-        <v>66</v>
-      </c>
-      <c r="H28" s="4">
-        <f t="shared" si="0"/>
-        <v>58.1</v>
-      </c>
+      <c r="B28" s="59"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="5">
-        <v>54</v>
-      </c>
-      <c r="D29" s="4">
-        <v>69</v>
-      </c>
-      <c r="E29" s="4">
-        <v>65</v>
-      </c>
-      <c r="F29" s="4">
-        <v>63</v>
-      </c>
-      <c r="G29" s="4">
-        <f t="shared" si="1"/>
-        <v>65.7</v>
-      </c>
-      <c r="H29" s="4">
-        <f t="shared" si="0"/>
-        <v>57.8</v>
-      </c>
+      <c r="B29" s="59"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="5">
-        <v>7</v>
-      </c>
-      <c r="D30" s="4">
-        <v>66</v>
-      </c>
-      <c r="E30" s="4">
-        <v>69</v>
-      </c>
-      <c r="F30" s="4">
-        <v>62</v>
-      </c>
-      <c r="G30" s="4">
-        <f t="shared" si="1"/>
-        <v>65.7</v>
-      </c>
-      <c r="H30" s="4">
-        <f t="shared" si="0"/>
-        <v>57.8</v>
-      </c>
+      <c r="B30" s="59"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="5">
-        <v>10</v>
-      </c>
-      <c r="D31" s="4">
-        <v>67</v>
-      </c>
-      <c r="E31" s="4">
-        <v>69</v>
-      </c>
-      <c r="F31" s="4">
-        <v>61</v>
-      </c>
-      <c r="G31" s="4">
-        <f t="shared" si="1"/>
-        <v>65.7</v>
-      </c>
-      <c r="H31" s="4">
-        <f t="shared" si="0"/>
-        <v>57.8</v>
-      </c>
+      <c r="B31" s="59"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="5">
-        <v>44</v>
-      </c>
-      <c r="D32" s="4">
-        <v>65</v>
-      </c>
-      <c r="E32" s="4">
-        <v>66</v>
-      </c>
-      <c r="F32" s="4">
-        <v>61</v>
-      </c>
-      <c r="G32" s="4">
-        <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="H32" s="4">
-        <f t="shared" si="0"/>
-        <v>56.3</v>
-      </c>
+      <c r="B32" s="59"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:H32">
@@ -3053,183 +2902,183 @@
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G2" s="27" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="13" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F3" s="17">
         <v>6</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="24"/>
       <c r="C4" s="29" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F4" s="18">
         <f>POWER(F3,1.15)</f>
         <v>7.8500773842522964</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="7" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="24"/>
       <c r="C5" s="29" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F5" s="18">
         <f t="shared" ref="F5:F7" si="0">POWER(F4,1.15)</f>
         <v>10.693134479003202</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="24"/>
       <c r="C6" s="29" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F6" s="18">
         <f t="shared" si="0"/>
         <v>15.257057498113838</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="31"/>
       <c r="C7" s="30" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F7" s="20">
         <f t="shared" si="0"/>
         <v>22.961031816314314</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="9" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F8" s="17">
         <v>5</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -3237,601 +3086,601 @@
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="24"/>
       <c r="C9" s="29" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F9" s="18">
         <f>POWER(F8,1.17)</f>
         <v>6.5734733273769663</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="24"/>
       <c r="C10" s="29" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F10" s="18">
         <f t="shared" ref="F10:F12" si="1">POWER(F9,1.17)</f>
         <v>9.0535736509971976</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="24"/>
       <c r="C11" s="29" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F11" s="18">
         <f t="shared" si="1"/>
         <v>13.166775950563464</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="7" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="24"/>
       <c r="C12" s="30" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F12" s="20">
         <f t="shared" si="1"/>
         <v>20.407553856606096</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F13" s="17">
         <v>5</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="24"/>
       <c r="C14" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="E14" s="29" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F14" s="18">
         <f>POWER(F13,1.12)</f>
         <v>6.0652178558631524</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="9" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="24"/>
       <c r="C15" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="E15" s="29" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F15" s="18">
         <f t="shared" ref="F15:F17" si="2">POWER(F14,1.12)</f>
         <v>7.529878583836755</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="24"/>
       <c r="C16" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="E16" s="29" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F16" s="18">
         <f t="shared" si="2"/>
         <v>9.5940622111548404</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="31"/>
       <c r="C17" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>58</v>
-      </c>
       <c r="E17" s="30" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F17" s="20">
         <f t="shared" si="2"/>
         <v>12.584699037675147</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F18" s="17">
         <v>8</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="24"/>
       <c r="C19" s="29" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F19" s="18">
         <f>POWER(F18,1.19)</f>
         <v>11.876188565032388</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="24"/>
       <c r="C20" s="29" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F20" s="18">
         <f t="shared" ref="F20:F22" si="3">POWER(F19,1.19)</f>
         <v>19.004906205455562</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="24"/>
       <c r="C21" s="29" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F21" s="18">
         <f t="shared" si="3"/>
         <v>33.254484458357737</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="24"/>
       <c r="C22" s="30" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F22" s="20">
         <f t="shared" si="3"/>
         <v>64.714523993093408</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F23" s="17">
         <v>4</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="24"/>
       <c r="C24" s="29" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F24" s="18">
         <f>POWER(F23,1.25)</f>
         <v>5.6568542494923806</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="24"/>
       <c r="C25" s="29" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F25" s="18">
         <f t="shared" ref="F25:F27" si="4">POWER(F24,1.25)</f>
         <v>8.7240618613220615</v>
       </c>
       <c r="G25" s="33" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="24"/>
       <c r="C26" s="29" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F26" s="18">
         <f t="shared" si="4"/>
         <v>14.993341072882401</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="31"/>
       <c r="C27" s="30" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F27" s="20">
         <f t="shared" si="4"/>
         <v>29.503465103338023</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="24" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F28" s="17">
         <v>10</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="24"/>
       <c r="C29" s="29" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F29" s="18">
         <f>POWER(F28,1.1)</f>
         <v>12.58925411794168</v>
       </c>
       <c r="G29" s="33" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="25"/>
       <c r="C30" s="29" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F30" s="18">
         <f t="shared" ref="F30:F32" si="5">POWER(F29,1.1)</f>
         <v>16.218100973589316</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="25"/>
       <c r="C31" s="29" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F31" s="18">
         <f t="shared" si="5"/>
         <v>21.428906011200613</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="25"/>
       <c r="C32" s="30" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F32" s="20">
         <f t="shared" si="5"/>
         <v>29.113874126187596</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="23" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F33" s="17">
         <v>20</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="25"/>
       <c r="C34" s="29" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="F34" s="18">
         <f>POWER(F33,1.05)</f>
         <v>23.231726992830843</v>
       </c>
       <c r="G34" s="33" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="25"/>
       <c r="C35" s="29" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F35" s="18">
         <f t="shared" ref="F35:F37" si="6">POWER(F34,1.05)</f>
         <v>27.188520168752266</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="25"/>
       <c r="C36" s="29" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F36" s="18">
         <f t="shared" si="6"/>
         <v>32.070434855082958</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="26"/>
       <c r="C37" s="30" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F37" s="20">
         <f t="shared" si="6"/>
         <v>38.142582228695794</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3861,47 +3710,47 @@
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="37" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C2" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>160</v>
-      </c>
-      <c r="F2" s="38" t="s">
+      <c r="G2" s="46" t="s">
         <v>165</v>
-      </c>
-      <c r="G2" s="46" t="s">
-        <v>173</v>
       </c>
       <c r="I2" s="44"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="39"/>
       <c r="C3" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="D3" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="D3" s="36" t="s">
-        <v>175</v>
-      </c>
       <c r="E3" s="40" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="G3" s="47" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="I3" s="45"/>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="48" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C4" s="49">
         <v>20</v>
@@ -3922,7 +3771,7 @@
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C5" s="49">
         <v>20</v>
@@ -3943,7 +3792,7 @@
     </row>
     <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="48" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C6" s="49">
         <v>18</v>
@@ -3964,7 +3813,7 @@
     </row>
     <row r="7" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="48" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C7" s="49">
         <v>11</v>
@@ -3985,7 +3834,7 @@
     </row>
     <row r="8" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="52" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C8" s="53">
         <v>19</v>
@@ -4006,16 +3855,16 @@
     </row>
     <row r="10" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="42" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="I10" s="57"/>
     </row>
@@ -4024,12 +3873,12 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="44" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="50" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C15">
         <f>ROUND((500*(C4/D4)+(E4/100)+(1/F4)),1)</f>
@@ -4038,7 +3887,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="50" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C16">
         <f t="shared" ref="C16:C19" si="0">ROUND((500*(C5/D5)+(E5/100)+(1/F5)),1)</f>
@@ -4047,7 +3896,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="50" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
@@ -4056,7 +3905,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="50" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
@@ -4065,7 +3914,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="50" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Added user selectable amount of races (for waiting times), and a score system that gets displayed automatically after the season, sorted by best driver
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\A2B-Project\Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
@@ -20,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drivers!$B$2:$H$32</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -57,9 +52,6 @@
     <t>Nicolas Hulkenberg</t>
   </si>
   <si>
-    <t>Sergio Perez Mendoza</t>
-  </si>
-  <si>
     <t>Kevin Magnussen</t>
   </si>
   <si>
@@ -84,9 +76,6 @@
     <t>Pascal Wehrlein</t>
   </si>
   <si>
-    <t>Esteban Ocon</t>
-  </si>
-  <si>
     <t>Romain Grosjean</t>
   </si>
   <si>
@@ -532,12 +521,18 @@
   </si>
   <si>
     <t>Track difficulty = 500/(Total Length / Amount of Turns)+(Max height diff / 100)+(1 / Longest straight)                      Scale of 1 to 5</t>
+  </si>
+  <si>
+    <t>Rio Haryanto</t>
+  </si>
+  <si>
+    <t>Sergio Perez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -1074,7 +1069,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1090,9 +1085,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1129,7 +1124,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1150,11 +1145,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="143898880"/>
-        <c:axId val="143904768"/>
+        <c:axId val="215795968"/>
+        <c:axId val="215801856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="143898880"/>
+        <c:axId val="215795968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1193,10 +1188,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143904768"/>
+        <c:crossAx val="215801856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1204,7 +1199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143904768"/>
+        <c:axId val="215801856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1251,10 +1246,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143898880"/>
+        <c:crossAx val="215795968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1292,7 +1287,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1862,7 +1857,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D42C97-3EA1-4707-94E5-704BAB9AF338}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{45D42C97-3EA1-4707-94E5-704BAB9AF338}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1886,9 +1881,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1926,9 +1921,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1961,26 +1956,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2013,26 +1991,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2209,7 +2170,7 @@
   <dimension ref="B2:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H32" sqref="B25:H32"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2228,22 +2189,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -2292,7 +2253,7 @@
         <v>95</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4:H32" si="0">(ROUND((G4/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" ref="H4:H24" si="0">(ROUND((G4/1.5)*1200000*1.1,-5))/1000000</f>
         <v>83.6</v>
       </c>
     </row>
@@ -2313,7 +2274,7 @@
         <v>95</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ref="G5:G32" si="1">ROUND(AVERAGE(D5:F5),1)</f>
+        <f t="shared" ref="G5:G24" si="1">ROUND(AVERAGE(D5:F5),1)</f>
         <v>94.7</v>
       </c>
       <c r="H5" s="4">
@@ -2398,7 +2359,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>168</v>
       </c>
       <c r="C9" s="5">
         <v>11</v>
@@ -2423,7 +2384,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="5">
         <v>14</v>
@@ -2498,7 +2459,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="5">
         <v>55</v>
@@ -2523,7 +2484,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="5">
         <v>20</v>
@@ -2573,7 +2534,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="5">
         <v>22</v>
@@ -2598,7 +2559,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="5">
         <v>12</v>
@@ -2623,7 +2584,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" s="5">
         <v>8</v>
@@ -2648,7 +2609,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="5">
         <v>94</v>
@@ -2673,7 +2634,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="5">
         <v>9</v>
@@ -2698,7 +2659,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="5">
         <v>26</v>
@@ -2723,7 +2684,7 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="5">
         <v>30</v>
@@ -2748,7 +2709,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>19</v>
+        <v>167</v>
       </c>
       <c r="C23" s="5">
         <v>34</v>
@@ -2773,7 +2734,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C24" s="5">
         <v>21</v>
@@ -2902,183 +2863,183 @@
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G2" s="27" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F3" s="17">
         <v>6</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="24"/>
       <c r="C4" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F4" s="18">
         <f>POWER(F3,1.15)</f>
         <v>7.8500773842522964</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="24"/>
       <c r="C5" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F5" s="18">
         <f t="shared" ref="F5:F7" si="0">POWER(F4,1.15)</f>
         <v>10.693134479003202</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="24"/>
       <c r="C6" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F6" s="18">
         <f t="shared" si="0"/>
         <v>15.257057498113838</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="31"/>
       <c r="C7" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F7" s="20">
         <f t="shared" si="0"/>
         <v>22.961031816314314</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F8" s="17">
         <v>5</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -3086,601 +3047,601 @@
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="24"/>
       <c r="C9" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F9" s="18">
         <f>POWER(F8,1.17)</f>
         <v>6.5734733273769663</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="24"/>
       <c r="C10" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F10" s="18">
         <f t="shared" ref="F10:F12" si="1">POWER(F9,1.17)</f>
         <v>9.0535736509971976</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="24"/>
       <c r="C11" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F11" s="18">
         <f t="shared" si="1"/>
         <v>13.166775950563464</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="24"/>
       <c r="C12" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F12" s="20">
         <f t="shared" si="1"/>
         <v>20.407553856606096</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F13" s="17">
         <v>5</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="24"/>
       <c r="C14" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F14" s="18">
         <f>POWER(F13,1.12)</f>
         <v>6.0652178558631524</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="24"/>
       <c r="C15" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F15" s="18">
         <f t="shared" ref="F15:F17" si="2">POWER(F14,1.12)</f>
         <v>7.529878583836755</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="24"/>
       <c r="C16" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" s="18">
         <f t="shared" si="2"/>
         <v>9.5940622111548404</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="31"/>
       <c r="C17" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F17" s="20">
         <f t="shared" si="2"/>
         <v>12.584699037675147</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F18" s="17">
         <v>8</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="24"/>
       <c r="C19" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F19" s="18">
         <f>POWER(F18,1.19)</f>
         <v>11.876188565032388</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="24"/>
       <c r="C20" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F20" s="18">
         <f t="shared" ref="F20:F22" si="3">POWER(F19,1.19)</f>
         <v>19.004906205455562</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="24"/>
       <c r="C21" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="29" t="s">
         <v>71</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>73</v>
       </c>
       <c r="F21" s="18">
         <f t="shared" si="3"/>
         <v>33.254484458357737</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="24"/>
       <c r="C22" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F22" s="20">
         <f t="shared" si="3"/>
         <v>64.714523993093408</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="28" t="s">
-        <v>36</v>
-      </c>
       <c r="D23" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F23" s="17">
         <v>4</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="24"/>
       <c r="C24" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F24" s="18">
         <f>POWER(F23,1.25)</f>
         <v>5.6568542494923806</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="24"/>
       <c r="C25" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F25" s="18">
         <f t="shared" ref="F25:F27" si="4">POWER(F24,1.25)</f>
         <v>8.7240618613220615</v>
       </c>
       <c r="G25" s="33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="24"/>
       <c r="C26" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F26" s="18">
         <f t="shared" si="4"/>
         <v>14.993341072882401</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="31"/>
       <c r="C27" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F27" s="20">
         <f t="shared" si="4"/>
         <v>29.503465103338023</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F28" s="17">
         <v>10</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="24"/>
       <c r="C29" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F29" s="18">
         <f>POWER(F28,1.1)</f>
         <v>12.58925411794168</v>
       </c>
       <c r="G29" s="33" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="25"/>
       <c r="C30" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F30" s="18">
         <f t="shared" ref="F30:F32" si="5">POWER(F29,1.1)</f>
         <v>16.218100973589316</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="25"/>
       <c r="C31" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F31" s="18">
         <f t="shared" si="5"/>
         <v>21.428906011200613</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="25"/>
       <c r="C32" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F32" s="20">
         <f t="shared" si="5"/>
         <v>29.113874126187596</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F33" s="17">
         <v>20</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="25"/>
       <c r="C34" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F34" s="18">
         <f>POWER(F33,1.05)</f>
         <v>23.231726992830843</v>
       </c>
       <c r="G34" s="33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="25"/>
       <c r="C35" s="29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F35" s="18">
         <f t="shared" ref="F35:F37" si="6">POWER(F34,1.05)</f>
         <v>27.188520168752266</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="25"/>
       <c r="C36" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E36" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F36" s="18">
         <f t="shared" si="6"/>
         <v>32.070434855082958</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="26"/>
       <c r="C37" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F37" s="20">
         <f t="shared" si="6"/>
         <v>38.142582228695794</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3710,47 +3671,47 @@
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="C2" s="41" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="38" t="s">
+      <c r="E2" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="E2" s="41" t="s">
-        <v>152</v>
-      </c>
       <c r="F2" s="38" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I2" s="44"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="39"/>
       <c r="C3" s="40" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G3" s="47" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I3" s="45"/>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="48" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C4" s="49">
         <v>20</v>
@@ -3771,7 +3732,7 @@
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" s="49">
         <v>20</v>
@@ -3792,7 +3753,7 @@
     </row>
     <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="48" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C6" s="49">
         <v>18</v>
@@ -3813,7 +3774,7 @@
     </row>
     <row r="7" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="48" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C7" s="49">
         <v>11</v>
@@ -3834,7 +3795,7 @@
     </row>
     <row r="8" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C8" s="53">
         <v>19</v>
@@ -3855,16 +3816,16 @@
     </row>
     <row r="10" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="F10" s="43" t="s">
         <v>162</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>164</v>
       </c>
       <c r="I10" s="57"/>
     </row>
@@ -3873,12 +3834,12 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="44" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="50" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C15">
         <f>ROUND((500*(C4/D4)+(E4/100)+(1/F4)),1)</f>
@@ -3887,7 +3848,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="50" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C16">
         <f t="shared" ref="C16:C19" si="0">ROUND((500*(C5/D5)+(E5/100)+(1/F5)),1)</f>
@@ -3896,7 +3857,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="50" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
@@ -3905,7 +3866,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
@@ -3914,7 +3875,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="50" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Added upgrades game data in json format
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BKuijpers\Documents\GitHub\A2B-Project\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Drivers" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drivers!$B$2:$H$32</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -262,21 +267,6 @@
     <t>Everything Level 5</t>
   </si>
   <si>
-    <t>Weight +1kg, Speed -1</t>
-  </si>
-  <si>
-    <t>Weight +1kg, Speed -2</t>
-  </si>
-  <si>
-    <t>Weight +1kg, Speed -3</t>
-  </si>
-  <si>
-    <t>Weight +1kg, Speed -4</t>
-  </si>
-  <si>
-    <t>Weight +1kg, Speed -5</t>
-  </si>
-  <si>
     <t>89/100</t>
   </si>
   <si>
@@ -527,12 +517,27 @@
   </si>
   <si>
     <t>Sergio Perez</t>
+  </si>
+  <si>
+    <t>Speed -2, Weight +1kg</t>
+  </si>
+  <si>
+    <t>Speed -3, Weight +1kg</t>
+  </si>
+  <si>
+    <t>Speed -4, Weight +1kg</t>
+  </si>
+  <si>
+    <t>Speed -5, Weight +1kg</t>
+  </si>
+  <si>
+    <t>Speed -1, Weight +1kg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -1085,7 +1090,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
@@ -1857,7 +1862,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{45D42C97-3EA1-4707-94E5-704BAB9AF338}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D42C97-3EA1-4707-94E5-704BAB9AF338}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1923,7 +1928,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1956,9 +1961,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1991,6 +2013,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -2169,7 +2208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2359,7 +2398,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C9" s="5">
         <v>11</v>
@@ -2709,7 +2748,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C23" s="5">
         <v>34</v>
@@ -2844,8 +2883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,7 +2914,7 @@
         <v>42</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G2" s="27" t="s">
         <v>0</v>
@@ -2899,7 +2938,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E3" s="28" t="s">
         <v>55</v>
@@ -2908,7 +2947,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="7" t="s">
@@ -2924,7 +2963,7 @@
         <v>37</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>56</v>
@@ -2934,7 +2973,7 @@
         <v>7.8500773842522964</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="7" t="s">
@@ -2950,7 +2989,7 @@
         <v>38</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>56</v>
@@ -2960,7 +2999,7 @@
         <v>10.693134479003202</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I5" s="11"/>
       <c r="J5" s="7" t="s">
@@ -2976,7 +3015,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E6" s="29" t="s">
         <v>57</v>
@@ -2986,7 +3025,7 @@
         <v>15.257057498113838</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="7" t="s">
@@ -3002,7 +3041,7 @@
         <v>40</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E7" s="30" t="s">
         <v>57</v>
@@ -3012,7 +3051,7 @@
         <v>22.961031816314314</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="9" t="s">
@@ -3033,13 +3072,13 @@
         <v>60</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F8" s="17">
         <v>5</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -3053,14 +3092,14 @@
         <v>61</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F9" s="18">
         <f>POWER(F8,1.17)</f>
         <v>6.5734733273769663</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>79</v>
@@ -3081,21 +3120,21 @@
         <v>62</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F10" s="18">
         <f t="shared" ref="F10:F12" si="1">POWER(F9,1.17)</f>
         <v>9.0535736509971976</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="7" t="s">
         <v>20</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
@@ -3107,21 +3146,21 @@
         <v>63</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F11" s="18">
         <f t="shared" si="1"/>
         <v>13.166775950563464</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="7" t="s">
         <v>21</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
@@ -3133,14 +3172,14 @@
         <v>64</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F12" s="20">
         <f t="shared" si="1"/>
         <v>20.407553856606096</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="7" t="s">
@@ -3167,14 +3206,14 @@
         <v>5</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="7" t="s">
         <v>52</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3193,14 +3232,14 @@
         <v>6.0652178558631524</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="9" t="s">
         <v>53</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
@@ -3219,7 +3258,7 @@
         <v>7.529878583836755</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
@@ -3238,7 +3277,7 @@
         <v>9.5940622111548404</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -3257,7 +3296,7 @@
         <v>12.584699037675147</v>
       </c>
       <c r="G17" s="30" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -3277,7 +3316,7 @@
         <v>8</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -3296,7 +3335,7 @@
         <v>11.876188565032388</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -3315,7 +3354,7 @@
         <v>19.004906205455562</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -3334,7 +3373,7 @@
         <v>33.254484458357737</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -3353,7 +3392,7 @@
         <v>64.714523993093408</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -3364,16 +3403,16 @@
         <v>34</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F23" s="17">
         <v>4</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
@@ -3382,17 +3421,17 @@
         <v>37</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F24" s="18">
         <f>POWER(F23,1.25)</f>
         <v>5.6568542494923806</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -3401,17 +3440,17 @@
         <v>38</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F25" s="18">
         <f t="shared" ref="F25:F27" si="4">POWER(F24,1.25)</f>
         <v>8.7240618613220615</v>
       </c>
       <c r="G25" s="33" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -3420,17 +3459,17 @@
         <v>39</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F26" s="18">
         <f t="shared" si="4"/>
         <v>14.993341072882401</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -3439,17 +3478,17 @@
         <v>40</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F27" s="20">
         <f t="shared" si="4"/>
         <v>29.503465103338023</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -3460,16 +3499,16 @@
         <v>34</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>80</v>
+        <v>168</v>
       </c>
       <c r="F28" s="17">
         <v>10</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -3478,17 +3517,17 @@
         <v>37</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
       <c r="F29" s="18">
         <f>POWER(F28,1.1)</f>
         <v>12.58925411794168</v>
       </c>
       <c r="G29" s="33" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
@@ -3497,17 +3536,17 @@
         <v>38</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>82</v>
+        <v>165</v>
       </c>
       <c r="F30" s="18">
         <f t="shared" ref="F30:F32" si="5">POWER(F29,1.1)</f>
         <v>16.218100973589316</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -3516,17 +3555,17 @@
         <v>39</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>83</v>
+        <v>166</v>
       </c>
       <c r="F31" s="18">
         <f t="shared" si="5"/>
         <v>21.428906011200613</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -3538,14 +3577,14 @@
         <v>72</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>84</v>
+        <v>167</v>
       </c>
       <c r="F32" s="20">
         <f t="shared" si="5"/>
         <v>29.113874126187596</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
@@ -3565,7 +3604,7 @@
         <v>20</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
@@ -3574,7 +3613,7 @@
         <v>37</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E34" s="29" t="s">
         <v>73</v>
@@ -3584,7 +3623,7 @@
         <v>23.231726992830843</v>
       </c>
       <c r="G34" s="33" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
@@ -3593,7 +3632,7 @@
         <v>38</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>76</v>
@@ -3603,7 +3642,7 @@
         <v>27.188520168752266</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -3612,7 +3651,7 @@
         <v>39</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E36" s="29" t="s">
         <v>77</v>
@@ -3622,7 +3661,7 @@
         <v>32.070434855082958</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -3631,7 +3670,7 @@
         <v>40</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E37" s="30" t="s">
         <v>78</v>
@@ -3641,7 +3680,7 @@
         <v>38.142582228695794</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3671,47 +3710,47 @@
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="37" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E2" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="F2" s="38" t="s">
-        <v>155</v>
-      </c>
       <c r="G2" s="46" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I2" s="44"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="39"/>
       <c r="C3" s="40" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G3" s="47" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I3" s="45"/>
     </row>
     <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="48" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C4" s="49">
         <v>20</v>
@@ -3732,7 +3771,7 @@
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="48" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C5" s="49">
         <v>20</v>
@@ -3753,7 +3792,7 @@
     </row>
     <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="48" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C6" s="49">
         <v>18</v>
@@ -3774,7 +3813,7 @@
     </row>
     <row r="7" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="48" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C7" s="49">
         <v>11</v>
@@ -3795,7 +3834,7 @@
     </row>
     <row r="8" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="52" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C8" s="53">
         <v>19</v>
@@ -3816,16 +3855,16 @@
     </row>
     <row r="10" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="42" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F10" s="43" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="I10" s="57"/>
     </row>
@@ -3834,12 +3873,12 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="44" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="50" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C15">
         <f>ROUND((500*(C4/D4)+(E4/100)+(1/F4)),1)</f>
@@ -3848,7 +3887,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="50" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C16">
         <f t="shared" ref="C16:C19" si="0">ROUND((500*(C5/D5)+(E5/100)+(1/F5)),1)</f>
@@ -3857,7 +3896,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="50" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
@@ -3866,7 +3905,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="50" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
@@ -3875,7 +3914,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="50" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Updated the game stats with all F1 tracks
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BKuijpers\Documents\GitHub\A2B-Project\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\A2B-Project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Drivers" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="184">
   <si>
     <t>Name</t>
   </si>
@@ -501,18 +501,9 @@
     <t>Track's with more speed will be faster on track's with longer straight tracks</t>
   </si>
   <si>
-    <t>Laps</t>
-  </si>
-  <si>
-    <t>Standard amount</t>
-  </si>
-  <si>
     <t>In meters</t>
   </si>
   <si>
-    <t>Track difficulty = 500/(Total Length / Amount of Turns)+(Max height diff / 100)+(1 / Longest straight)                      Scale of 1 to 5</t>
-  </si>
-  <si>
     <t>Rio Haryanto</t>
   </si>
   <si>
@@ -532,6 +523,60 @@
   </si>
   <si>
     <t>Speed -1, Weight +1kg</t>
+  </si>
+  <si>
+    <t>Melbourne Grand Prix Circuit, Australia</t>
+  </si>
+  <si>
+    <t>Bahrain International Circuit, Bahrain</t>
+  </si>
+  <si>
+    <t>Shanghai International Circuit, China</t>
+  </si>
+  <si>
+    <t>Sochi Autodrom, Russia</t>
+  </si>
+  <si>
+    <t>Circuit de Barcelona-Catalunya, Spain</t>
+  </si>
+  <si>
+    <t>Circuit Gilles Villeneuve, Canada</t>
+  </si>
+  <si>
+    <t>Red Bull Ring, Austria</t>
+  </si>
+  <si>
+    <t>Hungaroring, Hungaria</t>
+  </si>
+  <si>
+    <t>Hockenheimring, Germany</t>
+  </si>
+  <si>
+    <t>Marina Bay Street Circuit, Singapore</t>
+  </si>
+  <si>
+    <t>Sepang International Circuit, Malaysia</t>
+  </si>
+  <si>
+    <t>Suzuka International Racing Course, Japan</t>
+  </si>
+  <si>
+    <t>Circuit of the Americas, United States of America</t>
+  </si>
+  <si>
+    <t>Autódromo Hermanos Rodríguez, Mexico</t>
+  </si>
+  <si>
+    <t>Autódromo José Carlos Pace, Brazil</t>
+  </si>
+  <si>
+    <t>Yas Marina Circuit, United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Hungaroring, Hungary</t>
+  </si>
+  <si>
+    <t>Track difficulty = 500/(Total Length / Amount of Turns)+(Max height diff / 100)+(1 / Longest straight)-1                      Scale of 1 to 5</t>
   </si>
 </sst>
 </file>
@@ -589,7 +634,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -868,9 +913,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -881,33 +924,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -921,7 +938,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1032,49 +1049,67 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1092,7 +1127,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1129,7 +1164,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1193,7 +1228,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="215801856"/>
@@ -1251,7 +1286,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="215795968"/>
@@ -1292,7 +1327,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1845,7 +1880,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="94" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1856,7 +1891,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9310872" cy="6084186"/>
+    <xdr:ext cx="9291941" cy="6069654"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1886,9 +1921,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1926,7 +1961,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2032,7 +2067,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2398,7 +2433,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C9" s="5">
         <v>11</v>
@@ -2748,7 +2783,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C23" s="5">
         <v>34</v>
@@ -2797,7 +2832,7 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="59"/>
+      <c r="B25" s="53"/>
       <c r="C25" s="5"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -2806,7 +2841,7 @@
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="59"/>
+      <c r="B26" s="53"/>
       <c r="C26" s="5"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -2815,7 +2850,7 @@
       <c r="H26" s="7"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="59"/>
+      <c r="B27" s="53"/>
       <c r="C27" s="5"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -2824,7 +2859,7 @@
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="59"/>
+      <c r="B28" s="53"/>
       <c r="C28" s="5"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -2833,7 +2868,7 @@
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="59"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="5"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
@@ -2842,7 +2877,7 @@
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="59"/>
+      <c r="B30" s="53"/>
       <c r="C30" s="5"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
@@ -2851,7 +2886,7 @@
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="59"/>
+      <c r="B31" s="53"/>
       <c r="C31" s="5"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -2860,7 +2895,7 @@
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="59"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="5"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2883,7 +2918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
@@ -3502,7 +3537,7 @@
         <v>93</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F28" s="17">
         <v>10</v>
@@ -3520,7 +3555,7 @@
         <v>94</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F29" s="18">
         <f>POWER(F28,1.1)</f>
@@ -3539,7 +3574,7 @@
         <v>95</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F30" s="18">
         <f t="shared" ref="F30:F32" si="5">POWER(F29,1.1)</f>
@@ -3558,7 +3593,7 @@
         <v>96</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F31" s="18">
         <f t="shared" si="5"/>
@@ -3577,7 +3612,7 @@
         <v>72</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F32" s="20">
         <f t="shared" si="5"/>
@@ -3694,10 +3729,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I20"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3707,8 +3742,8 @@
     <col min="8" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="37" t="s">
         <v>141</v>
       </c>
@@ -3721,208 +3756,749 @@
       <c r="E2" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="46" t="s">
-        <v>158</v>
-      </c>
+      <c r="G2" s="62"/>
       <c r="I2" s="44"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="39"/>
       <c r="C3" s="40" t="s">
         <v>152</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E3" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="65" t="s">
         <v>144</v>
       </c>
-      <c r="G3" s="47" t="s">
-        <v>159</v>
-      </c>
+      <c r="G3" s="63"/>
       <c r="I3" s="45"/>
     </row>
-    <row r="4" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="48" t="s">
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="54">
+        <v>1</v>
+      </c>
+      <c r="B4" s="60" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="57">
+        <v>16</v>
+      </c>
+      <c r="D4" s="47">
+        <v>5303</v>
+      </c>
+      <c r="E4" s="57">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F4" s="55">
+        <v>0.8</v>
+      </c>
+      <c r="G4" s="47"/>
+      <c r="I4" s="50"/>
+    </row>
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="54">
+        <v>2</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="46">
+        <v>15</v>
+      </c>
+      <c r="D5" s="47">
+        <v>5412</v>
+      </c>
+      <c r="E5" s="46">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="F5" s="55">
+        <v>1.04</v>
+      </c>
+      <c r="G5" s="47"/>
+      <c r="I5" s="52"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="54">
+        <v>3</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="46">
+        <v>16</v>
+      </c>
+      <c r="D6" s="47">
+        <v>5451</v>
+      </c>
+      <c r="E6" s="46">
+        <v>7.4</v>
+      </c>
+      <c r="F6" s="55">
+        <v>1.2</v>
+      </c>
+      <c r="G6" s="47"/>
+      <c r="I6" s="52"/>
+    </row>
+    <row r="7" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="54">
+        <v>4</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="46">
+        <v>19</v>
+      </c>
+      <c r="D7" s="47">
+        <v>5848</v>
+      </c>
+      <c r="E7" s="46">
+        <v>1.9</v>
+      </c>
+      <c r="F7" s="55">
+        <v>0.7</v>
+      </c>
+      <c r="G7" s="47"/>
+      <c r="I7" s="52"/>
+    </row>
+    <row r="8" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="54">
+        <v>5</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="46">
+        <v>16</v>
+      </c>
+      <c r="D8" s="47">
+        <v>4655</v>
+      </c>
+      <c r="E8" s="46">
+        <v>29.6</v>
+      </c>
+      <c r="F8" s="55">
+        <v>1.05</v>
+      </c>
+      <c r="G8" s="47"/>
+      <c r="I8" s="52"/>
+    </row>
+    <row r="9" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="54">
+        <v>6</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="46">
+        <v>19</v>
+      </c>
+      <c r="D9" s="47">
+        <v>3337</v>
+      </c>
+      <c r="E9" s="46">
+        <v>42</v>
+      </c>
+      <c r="F9" s="55">
+        <v>0.47</v>
+      </c>
+      <c r="G9" s="47"/>
+    </row>
+    <row r="10" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="54">
+        <v>7</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>171</v>
+      </c>
+      <c r="C10" s="46">
+        <v>13</v>
+      </c>
+      <c r="D10" s="47">
+        <v>4361</v>
+      </c>
+      <c r="E10" s="46">
+        <v>5.2</v>
+      </c>
+      <c r="F10" s="55">
+        <v>0.67</v>
+      </c>
+      <c r="G10" s="47"/>
+      <c r="I10" s="51"/>
+    </row>
+    <row r="11" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="54">
+        <v>8</v>
+      </c>
+      <c r="B11" s="60" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C11" s="46">
         <v>20</v>
       </c>
-      <c r="D4" s="50">
+      <c r="D11" s="47">
         <v>6003</v>
       </c>
-      <c r="E4" s="49">
+      <c r="E11" s="46">
         <v>26.8</v>
       </c>
-      <c r="F4" s="50">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G4" s="51">
-        <v>51</v>
-      </c>
-      <c r="I4" s="56"/>
-    </row>
-    <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
+      <c r="F11" s="55">
+        <v>1.6</v>
+      </c>
+      <c r="G11" s="47"/>
+    </row>
+    <row r="12" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="54">
+        <v>9</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="46">
+        <v>9</v>
+      </c>
+      <c r="D12" s="47">
+        <v>4326</v>
+      </c>
+      <c r="E12" s="46">
+        <v>1.8</v>
+      </c>
+      <c r="F12" s="55">
+        <v>0.65</v>
+      </c>
+      <c r="G12" s="47"/>
+    </row>
+    <row r="13" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="54">
+        <v>10</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="46">
+        <v>18</v>
+      </c>
+      <c r="D13" s="47">
+        <v>5891</v>
+      </c>
+      <c r="E13" s="46">
+        <v>11.3</v>
+      </c>
+      <c r="F13" s="55">
+        <v>0.75</v>
+      </c>
+      <c r="G13" s="47"/>
+    </row>
+    <row r="14" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="54">
+        <v>11</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" s="46">
+        <v>14</v>
+      </c>
+      <c r="D14" s="47">
+        <v>4381</v>
+      </c>
+      <c r="E14" s="46">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="F14" s="55">
+        <v>0.8</v>
+      </c>
+      <c r="G14" s="47"/>
+    </row>
+    <row r="15" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="54">
+        <v>12</v>
+      </c>
+      <c r="B15" s="60" t="s">
+        <v>174</v>
+      </c>
+      <c r="C15" s="46">
+        <v>17</v>
+      </c>
+      <c r="D15" s="47">
+        <v>4574</v>
+      </c>
+      <c r="E15" s="46">
+        <v>4.3</v>
+      </c>
+      <c r="F15" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="47"/>
+    </row>
+    <row r="16" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="54">
+        <v>13</v>
+      </c>
+      <c r="B16" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C16" s="46">
         <v>20</v>
       </c>
-      <c r="D5" s="50">
+      <c r="D16" s="47">
         <v>7004</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E16" s="46">
         <v>102.2</v>
       </c>
-      <c r="F5" s="50">
-        <v>2.4</v>
-      </c>
-      <c r="G5" s="51">
-        <v>44</v>
-      </c>
-      <c r="I5" s="58"/>
-    </row>
-    <row r="6" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" s="49">
+      <c r="F16" s="55">
+        <v>0.77</v>
+      </c>
+      <c r="G16" s="47"/>
+    </row>
+    <row r="17" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="54">
+        <v>14</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="46">
+        <v>11</v>
+      </c>
+      <c r="D17" s="47">
+        <v>5793</v>
+      </c>
+      <c r="E17" s="46">
+        <v>12.8</v>
+      </c>
+      <c r="F17" s="55">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G17" s="47"/>
+    </row>
+    <row r="18" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="54">
+        <v>15</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="46">
+        <v>23</v>
+      </c>
+      <c r="D18" s="47">
+        <v>5065</v>
+      </c>
+      <c r="E18" s="46">
+        <v>5.3</v>
+      </c>
+      <c r="F18" s="55">
+        <v>1.2</v>
+      </c>
+      <c r="G18" s="47"/>
+    </row>
+    <row r="19" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="54">
+        <v>16</v>
+      </c>
+      <c r="B19" s="60" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="46">
+        <v>15</v>
+      </c>
+      <c r="D19" s="47">
+        <v>5543</v>
+      </c>
+      <c r="E19" s="46">
+        <v>22</v>
+      </c>
+      <c r="F19" s="55">
+        <v>0.9</v>
+      </c>
+      <c r="G19" s="47"/>
+    </row>
+    <row r="20" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="54">
+        <v>17</v>
+      </c>
+      <c r="B20" s="60" t="s">
+        <v>177</v>
+      </c>
+      <c r="C20" s="46">
+        <v>17</v>
+      </c>
+      <c r="D20" s="47">
+        <v>5807</v>
+      </c>
+      <c r="E20" s="46">
+        <v>40.4</v>
+      </c>
+      <c r="F20" s="55">
+        <v>0.75</v>
+      </c>
+      <c r="G20" s="47"/>
+    </row>
+    <row r="21" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="54">
         <v>18</v>
       </c>
-      <c r="D6" s="50">
-        <v>5891</v>
-      </c>
-      <c r="E6" s="49">
-        <v>11.3</v>
-      </c>
-      <c r="F6" s="50">
+      <c r="B21" s="60" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="46">
+        <v>20</v>
+      </c>
+      <c r="D21" s="47">
+        <v>3427</v>
+      </c>
+      <c r="E21" s="46">
+        <v>30.9</v>
+      </c>
+      <c r="F21" s="55">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G21" s="47"/>
+    </row>
+    <row r="22" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="54">
+        <v>19</v>
+      </c>
+      <c r="B22" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="46">
+        <v>17</v>
+      </c>
+      <c r="D22" s="47">
+        <v>4304</v>
+      </c>
+      <c r="E22" s="46">
+        <v>2.8</v>
+      </c>
+      <c r="F22" s="55">
+        <v>1.2</v>
+      </c>
+      <c r="G22" s="47"/>
+    </row>
+    <row r="23" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="54">
+        <v>20</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="46">
+        <v>15</v>
+      </c>
+      <c r="D23" s="47">
+        <v>4309</v>
+      </c>
+      <c r="E23" s="46">
+        <v>43</v>
+      </c>
+      <c r="F23" s="55">
+        <v>0.54</v>
+      </c>
+      <c r="G23" s="47"/>
+    </row>
+    <row r="24" spans="1:7" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="54">
+        <v>21</v>
+      </c>
+      <c r="B24" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="48">
+        <v>21</v>
+      </c>
+      <c r="D24" s="49">
+        <v>5554</v>
+      </c>
+      <c r="E24" s="48">
+        <v>10.7</v>
+      </c>
+      <c r="F24" s="56">
+        <v>1.2</v>
+      </c>
+      <c r="G24" s="47"/>
+    </row>
+    <row r="26" spans="1:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="C26" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="D26" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="F26" s="43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="44"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="44" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>1</v>
       </c>
-      <c r="G6" s="51">
-        <v>52</v>
-      </c>
-      <c r="I6" s="58"/>
-    </row>
-    <row r="7" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7" s="49">
-        <v>11</v>
-      </c>
-      <c r="D7" s="50">
-        <v>5793</v>
-      </c>
-      <c r="E7" s="49">
-        <v>12.8</v>
-      </c>
-      <c r="F7" s="50">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G7" s="51">
-        <v>53</v>
-      </c>
-      <c r="I7" s="58"/>
-    </row>
-    <row r="8" spans="2:9" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="52" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" s="53">
-        <v>19</v>
-      </c>
-      <c r="D8" s="54">
-        <v>3337</v>
-      </c>
-      <c r="E8" s="53">
-        <v>42</v>
-      </c>
-      <c r="F8" s="54">
-        <v>0.7</v>
-      </c>
-      <c r="G8" s="55">
-        <v>78</v>
-      </c>
-      <c r="I8" s="58"/>
-    </row>
-    <row r="10" spans="2:9" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>155</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="I10" s="57"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="44"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="44" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="50" t="s">
-        <v>153</v>
-      </c>
-      <c r="C15">
-        <f>ROUND((500*(C4/D4)+(E4/100)+(1/F4)),1)</f>
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="50" t="s">
-        <v>147</v>
-      </c>
-      <c r="C16">
-        <f t="shared" ref="C16:C19" si="0">ROUND((500*(C5/D5)+(E5/100)+(1/F5)),1)</f>
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="50" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17">
+      <c r="B31" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" s="58">
+        <f>ROUND((500*(C4/D4)+(E4/100)+(1/F4)),1)-1</f>
+        <v>1.7999999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" s="58">
+        <f t="shared" ref="C32:C51" si="0">ROUND((500*(C5/D5)+(E5/100)+(1/F5)),1)-1</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" s="58" t="s">
+        <v>168</v>
+      </c>
+      <c r="C33" s="58">
         <f t="shared" si="0"/>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="50" t="s">
-        <v>149</v>
-      </c>
-      <c r="C18">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="C34" s="58">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>5</v>
+      </c>
+      <c r="B35" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" s="58">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="50" t="s">
+    <row r="36" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>6</v>
+      </c>
+      <c r="B36" s="59" t="s">
         <v>151</v>
       </c>
-      <c r="C19">
+      <c r="C36" s="58">
         <f t="shared" si="0"/>
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="44"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="B37" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="C37" s="58">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>8</v>
+      </c>
+      <c r="B38" s="59" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="58">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>9</v>
+      </c>
+      <c r="B39" s="58" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" s="58">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>10</v>
+      </c>
+      <c r="B40" s="59" t="s">
+        <v>148</v>
+      </c>
+      <c r="C40" s="58">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>11</v>
+      </c>
+      <c r="B41" s="58" t="s">
+        <v>173</v>
+      </c>
+      <c r="C41" s="58">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>12</v>
+      </c>
+      <c r="B42" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" s="58">
+        <f t="shared" si="0"/>
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>13</v>
+      </c>
+      <c r="B43" s="59" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" s="58">
+        <f t="shared" si="0"/>
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>14</v>
+      </c>
+      <c r="B44" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" s="58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>15</v>
+      </c>
+      <c r="B45" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="C45" s="58">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>16</v>
+      </c>
+      <c r="B46" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="58">
+        <f t="shared" si="0"/>
+        <v>1.7000000000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>17</v>
+      </c>
+      <c r="B47" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" s="58">
+        <f t="shared" si="0"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>18</v>
+      </c>
+      <c r="B48" s="58" t="s">
+        <v>178</v>
+      </c>
+      <c r="C48" s="58">
+        <f t="shared" si="0"/>
+        <v>3.0999999999999996</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>19</v>
+      </c>
+      <c r="B49" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" s="58">
+        <f t="shared" si="0"/>
+        <v>1.7999999999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>20</v>
+      </c>
+      <c r="B50" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" s="58">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>21</v>
+      </c>
+      <c r="B51" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="C51" s="58">
+        <f t="shared" si="0"/>
+        <v>1.7999999999999998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tweaks with race. Fixed memory leak. Adjusted simulation without command line
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GitHub\A2B-Project\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikak\Documents\GitHub\A2B-Project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Drivers" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Chart1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drivers!$B$2:$H$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drivers!$B$2:$I$24</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="185">
   <si>
     <t>Name</t>
   </si>
@@ -577,6 +577,9 @@
   </si>
   <si>
     <t>Track difficulty = 500/(Total Length / Amount of Turns)+(Max height diff / 100)+(1 / Longest straight)-1                      Scale of 1 to 5</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -938,7 +941,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1107,9 +1110,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1127,7 +1136,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1164,7 +1173,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1228,7 +1237,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="215801856"/>
@@ -1286,7 +1295,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="215795968"/>
@@ -1327,7 +1336,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1921,9 +1930,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1961,7 +1970,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2067,7 +2076,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2241,55 +2250,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H32"/>
+  <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="66">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5">
+      <c r="D3" s="5">
         <v>33</v>
-      </c>
-      <c r="D3" s="4">
-        <v>96</v>
       </c>
       <c r="E3" s="4">
         <v>96</v>
@@ -2298,73 +2311,82 @@
         <v>96</v>
       </c>
       <c r="G3" s="4">
-        <f>ROUND(AVERAGE(D3:F3),1)</f>
         <v>96</v>
       </c>
       <c r="H3" s="4">
-        <f>(ROUND((G3/1.5)*1200000*1.1,-5))/1000000</f>
+        <f>ROUND(AVERAGE(E3:G3),1)</f>
+        <v>96</v>
+      </c>
+      <c r="I3" s="4">
+        <f>(ROUND((H3/1.5)*1200000*1.1,-5))/1000000</f>
         <v>84.5</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="66">
         <v>2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5">
         <v>6</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>97</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>95</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>93</v>
       </c>
-      <c r="G4" s="4">
-        <f>ROUND(AVERAGE(D4:F4),1)</f>
+      <c r="H4" s="4">
+        <f>ROUND(AVERAGE(E4:G4),1)</f>
         <v>95</v>
       </c>
-      <c r="H4" s="4">
-        <f t="shared" ref="H4:H24" si="0">(ROUND((G4/1.5)*1200000*1.1,-5))/1000000</f>
+      <c r="I4" s="4">
+        <f>(ROUND((H4/1.5)*1200000*1.1,-5))/1000000</f>
         <v>83.6</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="66">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
+      <c r="D5" s="5">
         <v>44</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>94</v>
-      </c>
-      <c r="E5" s="4">
-        <v>95</v>
       </c>
       <c r="F5" s="4">
         <v>95</v>
       </c>
       <c r="G5" s="4">
-        <f t="shared" ref="G5:G24" si="1">ROUND(AVERAGE(D5:F5),1)</f>
+        <v>95</v>
+      </c>
+      <c r="H5" s="4">
+        <f>ROUND(AVERAGE(E5:G5),1)</f>
         <v>94.7</v>
       </c>
-      <c r="H5" s="4">
-        <f t="shared" si="0"/>
+      <c r="I5" s="4">
+        <f>(ROUND((H5/1.5)*1200000*1.1,-5))/1000000</f>
         <v>83.3</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="66">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5">
+      <c r="D6" s="5">
         <v>5</v>
-      </c>
-      <c r="D6" s="4">
-        <v>94</v>
       </c>
       <c r="E6" s="4">
         <v>94</v>
@@ -2373,540 +2395,597 @@
         <v>94</v>
       </c>
       <c r="G6" s="4">
-        <f t="shared" si="1"/>
         <v>94</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="0"/>
+        <f>ROUND(AVERAGE(E6:G6),1)</f>
+        <v>94</v>
+      </c>
+      <c r="I6" s="4">
+        <f>(ROUND((H6/1.5)*1200000*1.1,-5))/1000000</f>
         <v>82.7</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="66">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5">
+      <c r="D7" s="5">
         <v>3</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <v>93</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>94</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>90</v>
       </c>
-      <c r="G7" s="4">
-        <f t="shared" si="1"/>
+      <c r="H7" s="4">
+        <f>ROUND(AVERAGE(E7:G7),1)</f>
         <v>92.3</v>
       </c>
-      <c r="H7" s="4">
-        <f t="shared" si="0"/>
+      <c r="I7" s="4">
+        <f>(ROUND((H7/1.5)*1200000*1.1,-5))/1000000</f>
         <v>81.2</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="66">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5">
+      <c r="D8" s="5">
         <v>7</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <v>92</v>
-      </c>
-      <c r="E8" s="4">
-        <v>90</v>
       </c>
       <c r="F8" s="4">
         <v>90</v>
       </c>
       <c r="G8" s="4">
-        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="H8" s="4">
+        <f>ROUND(AVERAGE(E8:G8),1)</f>
         <v>90.7</v>
       </c>
-      <c r="H8" s="4">
-        <f t="shared" si="0"/>
+      <c r="I8" s="4">
+        <f>(ROUND((H8/1.5)*1200000*1.1,-5))/1000000</f>
         <v>79.8</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="66">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C9" s="5">
+      <c r="D9" s="5">
         <v>11</v>
-      </c>
-      <c r="D9" s="4">
-        <v>86</v>
       </c>
       <c r="E9" s="4">
         <v>86</v>
       </c>
       <c r="F9" s="4">
+        <v>86</v>
+      </c>
+      <c r="G9" s="4">
         <v>85</v>
       </c>
-      <c r="G9" s="4">
-        <f t="shared" si="1"/>
+      <c r="H9" s="4">
+        <f>ROUND(AVERAGE(E9:G9),1)</f>
         <v>85.7</v>
       </c>
-      <c r="H9" s="4">
-        <f t="shared" si="0"/>
+      <c r="I9" s="4">
+        <f>(ROUND((H9/1.5)*1200000*1.1,-5))/1000000</f>
         <v>75.400000000000006</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="66">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5">
+      <c r="D10" s="5">
         <v>14</v>
-      </c>
-      <c r="D10" s="4">
-        <v>85</v>
       </c>
       <c r="E10" s="4">
         <v>85</v>
       </c>
       <c r="F10" s="4">
+        <v>85</v>
+      </c>
+      <c r="G10" s="4">
         <v>82</v>
       </c>
-      <c r="G10" s="4">
-        <f t="shared" si="1"/>
+      <c r="H10" s="4">
+        <f>ROUND(AVERAGE(E10:G10),1)</f>
         <v>84</v>
       </c>
-      <c r="H10" s="4">
-        <f t="shared" si="0"/>
+      <c r="I10" s="4">
+        <f>(ROUND((H10/1.5)*1200000*1.1,-5))/1000000</f>
         <v>73.900000000000006</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="66">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="5">
+      <c r="D11" s="5">
         <v>77</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <v>80</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="4">
         <v>84</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <v>83</v>
       </c>
-      <c r="G11" s="4">
-        <f t="shared" si="1"/>
+      <c r="H11" s="4">
+        <f>ROUND(AVERAGE(E11:G11),1)</f>
         <v>82.3</v>
       </c>
-      <c r="H11" s="4">
-        <f t="shared" si="0"/>
+      <c r="I11" s="4">
+        <f>(ROUND((H11/1.5)*1200000*1.1,-5))/1000000</f>
         <v>72.400000000000006</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="66">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5">
+      <c r="D12" s="5">
         <v>27</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="4">
         <v>82</v>
       </c>
-      <c r="E12" s="4">
+      <c r="F12" s="4">
         <v>75</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <v>82</v>
       </c>
-      <c r="G12" s="4">
-        <f t="shared" si="1"/>
+      <c r="H12" s="4">
+        <f>ROUND(AVERAGE(E12:G12),1)</f>
         <v>79.7</v>
       </c>
-      <c r="H12" s="4">
-        <f t="shared" si="0"/>
+      <c r="I12" s="4">
+        <f>(ROUND((H12/1.5)*1200000*1.1,-5))/1000000</f>
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="66">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="5">
+      <c r="D13" s="5">
         <v>55</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="4">
         <v>81</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="4">
         <v>74</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="4">
         <v>82</v>
       </c>
-      <c r="G13" s="4">
-        <f t="shared" si="1"/>
+      <c r="H13" s="4">
+        <f>ROUND(AVERAGE(E13:G13),1)</f>
         <v>79</v>
       </c>
-      <c r="H13" s="4">
-        <f t="shared" si="0"/>
+      <c r="I13" s="4">
+        <f>(ROUND((H13/1.5)*1200000*1.1,-5))/1000000</f>
         <v>69.5</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="66">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="5">
+      <c r="D14" s="5">
         <v>20</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E14" s="4">
         <v>76</v>
       </c>
-      <c r="E14" s="4">
+      <c r="F14" s="4">
         <v>82</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G14" s="4">
         <v>78</v>
       </c>
-      <c r="G14" s="4">
-        <f t="shared" si="1"/>
+      <c r="H14" s="4">
+        <f>ROUND(AVERAGE(E14:G14),1)</f>
         <v>78.7</v>
       </c>
-      <c r="H14" s="4">
-        <f t="shared" si="0"/>
+      <c r="I14" s="4">
+        <f>(ROUND((H14/1.5)*1200000*1.1,-5))/1000000</f>
         <v>69.3</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="66">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="5">
+      <c r="D15" s="5">
         <v>19</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="4">
         <v>80</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F15" s="4">
         <v>78</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="4">
         <v>75</v>
       </c>
-      <c r="G15" s="4">
-        <f t="shared" si="1"/>
+      <c r="H15" s="4">
+        <f>ROUND(AVERAGE(E15:G15),1)</f>
         <v>77.7</v>
       </c>
-      <c r="H15" s="4">
-        <f t="shared" si="0"/>
+      <c r="I15" s="4">
+        <f>(ROUND((H15/1.5)*1200000*1.1,-5))/1000000</f>
         <v>68.400000000000006</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="66">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="5">
+      <c r="D16" s="5">
         <v>22</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="4">
         <v>78</v>
       </c>
-      <c r="E16" s="4">
+      <c r="F16" s="4">
         <v>74</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
         <v>80</v>
       </c>
-      <c r="G16" s="4">
-        <f t="shared" si="1"/>
+      <c r="H16" s="4">
+        <f>ROUND(AVERAGE(E16:G16),1)</f>
         <v>77.3</v>
       </c>
-      <c r="H16" s="4">
-        <f t="shared" si="0"/>
+      <c r="I16" s="4">
+        <f>(ROUND((H16/1.5)*1200000*1.1,-5))/1000000</f>
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="66">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="5">
+      <c r="D17" s="5">
         <v>12</v>
-      </c>
-      <c r="D17" s="4">
-        <v>76</v>
       </c>
       <c r="E17" s="4">
         <v>76</v>
       </c>
       <c r="F17" s="4">
+        <v>76</v>
+      </c>
+      <c r="G17" s="4">
         <v>79</v>
       </c>
-      <c r="G17" s="4">
-        <f t="shared" si="1"/>
+      <c r="H17" s="4">
+        <f>ROUND(AVERAGE(E17:G17),1)</f>
         <v>77</v>
       </c>
-      <c r="H17" s="4">
-        <f t="shared" si="0"/>
+      <c r="I17" s="4">
+        <f>(ROUND((H17/1.5)*1200000*1.1,-5))/1000000</f>
         <v>67.8</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="66">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="5">
+      <c r="D18" s="5">
         <v>8</v>
       </c>
-      <c r="D18" s="4">
+      <c r="E18" s="4">
         <v>79</v>
       </c>
-      <c r="E18" s="4">
+      <c r="F18" s="4">
         <v>76</v>
       </c>
-      <c r="F18" s="4">
+      <c r="G18" s="4">
         <v>75</v>
       </c>
-      <c r="G18" s="4">
-        <f t="shared" si="1"/>
+      <c r="H18" s="4">
+        <f>ROUND(AVERAGE(E18:G18),1)</f>
         <v>76.7</v>
       </c>
-      <c r="H18" s="4">
-        <f t="shared" si="0"/>
+      <c r="I18" s="4">
+        <f>(ROUND((H18/1.5)*1200000*1.1,-5))/1000000</f>
         <v>67.5</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="66">
         <v>17</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="5">
         <v>94</v>
       </c>
-      <c r="D19" s="4">
+      <c r="E19" s="4">
         <v>74</v>
       </c>
-      <c r="E19" s="4">
+      <c r="F19" s="4">
         <v>78</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
         <v>74</v>
       </c>
-      <c r="G19" s="4">
-        <f t="shared" si="1"/>
+      <c r="H19" s="4">
+        <f>ROUND(AVERAGE(E19:G19),1)</f>
         <v>75.3</v>
       </c>
-      <c r="H19" s="4">
-        <f t="shared" si="0"/>
+      <c r="I19" s="4">
+        <f>(ROUND((H19/1.5)*1200000*1.1,-5))/1000000</f>
         <v>66.3</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="66">
+        <v>18</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="5">
+      <c r="D20" s="5">
         <v>9</v>
       </c>
-      <c r="D20" s="4">
+      <c r="E20" s="4">
         <v>72</v>
       </c>
-      <c r="E20" s="4">
+      <c r="F20" s="4">
         <v>82</v>
       </c>
-      <c r="F20" s="4">
+      <c r="G20" s="4">
         <v>71</v>
       </c>
-      <c r="G20" s="4">
-        <f t="shared" si="1"/>
+      <c r="H20" s="4">
+        <f>ROUND(AVERAGE(E20:G20),1)</f>
         <v>75</v>
       </c>
-      <c r="H20" s="4">
-        <f t="shared" si="0"/>
+      <c r="I20" s="4">
+        <f>(ROUND((H20/1.5)*1200000*1.1,-5))/1000000</f>
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="66">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="5">
+      <c r="D21" s="5">
         <v>26</v>
       </c>
-      <c r="D21" s="4">
+      <c r="E21" s="4">
         <v>78</v>
       </c>
-      <c r="E21" s="4">
+      <c r="F21" s="4">
         <v>70</v>
       </c>
-      <c r="F21" s="4">
+      <c r="G21" s="4">
         <v>74</v>
       </c>
-      <c r="G21" s="4">
-        <f t="shared" si="1"/>
+      <c r="H21" s="4">
+        <f>ROUND(AVERAGE(E21:G21),1)</f>
         <v>74</v>
       </c>
-      <c r="H21" s="4">
-        <f t="shared" si="0"/>
+      <c r="I21" s="4">
+        <f>(ROUND((H21/1.5)*1200000*1.1,-5))/1000000</f>
         <v>65.099999999999994</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="66">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="5">
+      <c r="D22" s="5">
         <v>30</v>
       </c>
-      <c r="D22" s="4">
+      <c r="E22" s="4">
         <v>73</v>
       </c>
-      <c r="E22" s="4">
+      <c r="F22" s="4">
         <v>72</v>
       </c>
-      <c r="F22" s="4">
+      <c r="G22" s="4">
         <v>71</v>
       </c>
-      <c r="G22" s="4">
-        <f t="shared" si="1"/>
+      <c r="H22" s="4">
+        <f>ROUND(AVERAGE(E22:G22),1)</f>
         <v>72</v>
       </c>
-      <c r="H22" s="4">
-        <f t="shared" si="0"/>
+      <c r="I22" s="4">
+        <f>(ROUND((H22/1.5)*1200000*1.1,-5))/1000000</f>
         <v>63.4</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="66">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C23" s="5">
+      <c r="D23" s="5">
         <v>34</v>
       </c>
-      <c r="D23" s="4">
+      <c r="E23" s="4">
         <v>71</v>
       </c>
-      <c r="E23" s="4">
+      <c r="F23" s="4">
         <v>70</v>
       </c>
-      <c r="F23" s="4">
+      <c r="G23" s="4">
         <v>72</v>
       </c>
-      <c r="G23" s="4">
-        <f t="shared" si="1"/>
+      <c r="H23" s="4">
+        <f>ROUND(AVERAGE(E23:G23),1)</f>
         <v>71</v>
       </c>
-      <c r="H23" s="4">
-        <f t="shared" si="0"/>
+      <c r="I23" s="4">
+        <f>(ROUND((H23/1.5)*1200000*1.1,-5))/1000000</f>
         <v>62.5</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="67">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="5">
+      <c r="D24" s="5">
         <v>21</v>
       </c>
-      <c r="D24" s="4">
+      <c r="E24" s="4">
         <v>72</v>
-      </c>
-      <c r="E24" s="4">
-        <v>69</v>
       </c>
       <c r="F24" s="4">
         <v>69</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="H24" s="4">
+        <f>ROUND(AVERAGE(E24:G24),1)</f>
         <v>70</v>
       </c>
-      <c r="H24" s="4">
-        <f t="shared" si="0"/>
+      <c r="I24" s="4">
+        <f>(ROUND((H24/1.5)*1200000*1.1,-5))/1000000</f>
         <v>61.6</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="53"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="7"/>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="53"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="53"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="7"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="53"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="53"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="7"/>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="53"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="53"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="7"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="53"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="53"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="7"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="53"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="53"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="7"/>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="53"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="53"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="7"/>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="53"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="53"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="7"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="53"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H32">
-    <sortState ref="B3:H32">
-      <sortCondition descending="1" ref="G2:G32"/>
+  <autoFilter ref="B2:I24">
+    <sortState ref="B3:I24">
+      <sortCondition ref="B2:B24"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3731,7 +3810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added points to Driver object, will read from json. Updated game data for all driver and team id's.
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Drivers" sheetId="1" r:id="rId1"/>
     <sheet name="Car Upgrades" sheetId="2" r:id="rId2"/>
     <sheet name="Race Time Calculation" sheetId="3" r:id="rId3"/>
-    <sheet name="Chart1" sheetId="4" r:id="rId4"/>
+    <sheet name="ID's" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drivers!$B$2:$I$24</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="199">
   <si>
     <t>Name</t>
   </si>
@@ -580,6 +580,48 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>Driver ID</t>
+  </si>
+  <si>
+    <t>Team ID</t>
+  </si>
+  <si>
+    <t>Ferrari</t>
+  </si>
+  <si>
+    <t>Force India</t>
+  </si>
+  <si>
+    <t>Haas</t>
+  </si>
+  <si>
+    <t>Manor</t>
+  </si>
+  <si>
+    <t>McLaren</t>
+  </si>
+  <si>
+    <t>Mercedes</t>
+  </si>
+  <si>
+    <t>Red Bull</t>
+  </si>
+  <si>
+    <t>Renault</t>
+  </si>
+  <si>
+    <t>Sauber</t>
+  </si>
+  <si>
+    <t>Toro Rosso</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max Verstappen  </t>
   </si>
 </sst>
 </file>
@@ -637,7 +679,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -937,11 +979,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1116,6 +1189,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1131,802 +1215,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="nl-NL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="215795968"/>
-        <c:axId val="215801856"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="215795968"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="215801856"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="215801856"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="215795968"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9291941" cy="6069654"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D42C97-3EA1-4707-94E5-704BAB9AF338}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2252,8 +1540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2314,11 +1602,11 @@
         <v>96</v>
       </c>
       <c r="H3" s="4">
-        <f>ROUND(AVERAGE(E3:G3),1)</f>
+        <f t="shared" ref="H3:H24" si="0">ROUND(AVERAGE(E3:G3),1)</f>
         <v>96</v>
       </c>
       <c r="I3" s="4">
-        <f>(ROUND((H3/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" ref="I3:I24" si="1">(ROUND((H3/1.5)*1200000*1.1,-5))/1000000</f>
         <v>84.5</v>
       </c>
     </row>
@@ -2342,11 +1630,11 @@
         <v>93</v>
       </c>
       <c r="H4" s="4">
-        <f>ROUND(AVERAGE(E4:G4),1)</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="I4" s="4">
-        <f>(ROUND((H4/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>83.6</v>
       </c>
     </row>
@@ -2370,11 +1658,11 @@
         <v>95</v>
       </c>
       <c r="H5" s="4">
-        <f>ROUND(AVERAGE(E5:G5),1)</f>
+        <f t="shared" si="0"/>
         <v>94.7</v>
       </c>
       <c r="I5" s="4">
-        <f>(ROUND((H5/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>83.3</v>
       </c>
     </row>
@@ -2398,11 +1686,11 @@
         <v>94</v>
       </c>
       <c r="H6" s="4">
-        <f>ROUND(AVERAGE(E6:G6),1)</f>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="I6" s="4">
-        <f>(ROUND((H6/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>82.7</v>
       </c>
     </row>
@@ -2426,11 +1714,11 @@
         <v>90</v>
       </c>
       <c r="H7" s="4">
-        <f>ROUND(AVERAGE(E7:G7),1)</f>
+        <f t="shared" si="0"/>
         <v>92.3</v>
       </c>
       <c r="I7" s="4">
-        <f>(ROUND((H7/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>81.2</v>
       </c>
     </row>
@@ -2454,11 +1742,11 @@
         <v>90</v>
       </c>
       <c r="H8" s="4">
-        <f>ROUND(AVERAGE(E8:G8),1)</f>
+        <f t="shared" si="0"/>
         <v>90.7</v>
       </c>
       <c r="I8" s="4">
-        <f>(ROUND((H8/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>79.8</v>
       </c>
     </row>
@@ -2482,11 +1770,11 @@
         <v>85</v>
       </c>
       <c r="H9" s="4">
-        <f>ROUND(AVERAGE(E9:G9),1)</f>
+        <f t="shared" si="0"/>
         <v>85.7</v>
       </c>
       <c r="I9" s="4">
-        <f>(ROUND((H9/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>75.400000000000006</v>
       </c>
     </row>
@@ -2510,11 +1798,11 @@
         <v>82</v>
       </c>
       <c r="H10" s="4">
-        <f>ROUND(AVERAGE(E10:G10),1)</f>
+        <f t="shared" si="0"/>
         <v>84</v>
       </c>
       <c r="I10" s="4">
-        <f>(ROUND((H10/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>73.900000000000006</v>
       </c>
     </row>
@@ -2538,11 +1826,11 @@
         <v>83</v>
       </c>
       <c r="H11" s="4">
-        <f>ROUND(AVERAGE(E11:G11),1)</f>
+        <f t="shared" si="0"/>
         <v>82.3</v>
       </c>
       <c r="I11" s="4">
-        <f>(ROUND((H11/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>72.400000000000006</v>
       </c>
     </row>
@@ -2566,11 +1854,11 @@
         <v>82</v>
       </c>
       <c r="H12" s="4">
-        <f>ROUND(AVERAGE(E12:G12),1)</f>
+        <f t="shared" si="0"/>
         <v>79.7</v>
       </c>
       <c r="I12" s="4">
-        <f>(ROUND((H12/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>70.099999999999994</v>
       </c>
     </row>
@@ -2594,11 +1882,11 @@
         <v>82</v>
       </c>
       <c r="H13" s="4">
-        <f>ROUND(AVERAGE(E13:G13),1)</f>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="I13" s="4">
-        <f>(ROUND((H13/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>69.5</v>
       </c>
     </row>
@@ -2622,11 +1910,11 @@
         <v>78</v>
       </c>
       <c r="H14" s="4">
-        <f>ROUND(AVERAGE(E14:G14),1)</f>
+        <f t="shared" si="0"/>
         <v>78.7</v>
       </c>
       <c r="I14" s="4">
-        <f>(ROUND((H14/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>69.3</v>
       </c>
     </row>
@@ -2650,11 +1938,11 @@
         <v>75</v>
       </c>
       <c r="H15" s="4">
-        <f>ROUND(AVERAGE(E15:G15),1)</f>
+        <f t="shared" si="0"/>
         <v>77.7</v>
       </c>
       <c r="I15" s="4">
-        <f>(ROUND((H15/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>68.400000000000006</v>
       </c>
     </row>
@@ -2678,11 +1966,11 @@
         <v>80</v>
       </c>
       <c r="H16" s="4">
-        <f>ROUND(AVERAGE(E16:G16),1)</f>
+        <f t="shared" si="0"/>
         <v>77.3</v>
       </c>
       <c r="I16" s="4">
-        <f>(ROUND((H16/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>68</v>
       </c>
     </row>
@@ -2706,11 +1994,11 @@
         <v>79</v>
       </c>
       <c r="H17" s="4">
-        <f>ROUND(AVERAGE(E17:G17),1)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="I17" s="4">
-        <f>(ROUND((H17/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>67.8</v>
       </c>
     </row>
@@ -2734,11 +2022,11 @@
         <v>75</v>
       </c>
       <c r="H18" s="4">
-        <f>ROUND(AVERAGE(E18:G18),1)</f>
+        <f t="shared" si="0"/>
         <v>76.7</v>
       </c>
       <c r="I18" s="4">
-        <f>(ROUND((H18/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>67.5</v>
       </c>
     </row>
@@ -2762,11 +2050,11 @@
         <v>74</v>
       </c>
       <c r="H19" s="4">
-        <f>ROUND(AVERAGE(E19:G19),1)</f>
+        <f t="shared" si="0"/>
         <v>75.3</v>
       </c>
       <c r="I19" s="4">
-        <f>(ROUND((H19/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>66.3</v>
       </c>
     </row>
@@ -2790,11 +2078,11 @@
         <v>71</v>
       </c>
       <c r="H20" s="4">
-        <f>ROUND(AVERAGE(E20:G20),1)</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="I20" s="4">
-        <f>(ROUND((H20/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
     </row>
@@ -2818,11 +2106,11 @@
         <v>74</v>
       </c>
       <c r="H21" s="4">
-        <f>ROUND(AVERAGE(E21:G21),1)</f>
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="I21" s="4">
-        <f>(ROUND((H21/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>65.099999999999994</v>
       </c>
     </row>
@@ -2846,11 +2134,11 @@
         <v>71</v>
       </c>
       <c r="H22" s="4">
-        <f>ROUND(AVERAGE(E22:G22),1)</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="I22" s="4">
-        <f>(ROUND((H22/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>63.4</v>
       </c>
     </row>
@@ -2874,11 +2162,11 @@
         <v>72</v>
       </c>
       <c r="H23" s="4">
-        <f>ROUND(AVERAGE(E23:G23),1)</f>
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="I23" s="4">
-        <f>(ROUND((H23/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>62.5</v>
       </c>
     </row>
@@ -2902,11 +2190,11 @@
         <v>69</v>
       </c>
       <c r="H24" s="4">
-        <f>ROUND(AVERAGE(E24:G24),1)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="I24" s="4">
-        <f>(ROUND((H24/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>61.6</v>
       </c>
     </row>
@@ -4582,4 +3870,304 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="70" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="68">
+        <v>1</v>
+      </c>
+      <c r="C3" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="66">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="68">
+        <v>2</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="66">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="68">
+        <v>3</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="66">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="68">
+        <v>4</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="66">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="68">
+        <v>5</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="66">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="68">
+        <v>6</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="66">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="68">
+        <v>7</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="66">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="68">
+        <v>8</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="66">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="68">
+        <v>9</v>
+      </c>
+      <c r="C11" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="66">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="68">
+        <v>10</v>
+      </c>
+      <c r="C12" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="66">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="68">
+        <v>11</v>
+      </c>
+      <c r="C13" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="66">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="68">
+        <v>12</v>
+      </c>
+      <c r="C14" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="68"/>
+      <c r="F14" s="53"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="68">
+        <v>13</v>
+      </c>
+      <c r="C15" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="68"/>
+      <c r="F15" s="53"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="68">
+        <v>14</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="68"/>
+      <c r="F16" s="53"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="68">
+        <v>15</v>
+      </c>
+      <c r="C17" s="73" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="68"/>
+      <c r="F17" s="53"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="68">
+        <v>16</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="68"/>
+      <c r="F18" s="53"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="68">
+        <v>17</v>
+      </c>
+      <c r="C19" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="68"/>
+      <c r="F19" s="53"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="68">
+        <v>18</v>
+      </c>
+      <c r="C20" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="68"/>
+      <c r="F20" s="53"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="68">
+        <v>19</v>
+      </c>
+      <c r="C21" s="73" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="68"/>
+      <c r="F21" s="53"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="68">
+        <v>20</v>
+      </c>
+      <c r="C22" s="73" t="s">
+        <v>198</v>
+      </c>
+      <c r="E22" s="68"/>
+      <c r="F22" s="53"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="68">
+        <v>21</v>
+      </c>
+      <c r="C23" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="68"/>
+      <c r="F23" s="53"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="69">
+        <v>22</v>
+      </c>
+      <c r="C24" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="69"/>
+      <c r="F24" s="53"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
After race, all driver points are added and stored in json file. The drivers are read from a JSON file and stored in the profile. Standings screen read from drivers JSON file and will display the correct amount of points for each driver. On start game all driver points are reset, not on resume.
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Drivers" sheetId="1" r:id="rId1"/>
-    <sheet name="Car Upgrades" sheetId="2" r:id="rId2"/>
-    <sheet name="Race Time Calculation" sheetId="3" r:id="rId3"/>
-    <sheet name="ID's" sheetId="5" r:id="rId4"/>
+    <sheet name="ID's" sheetId="5" r:id="rId2"/>
+    <sheet name="Car Upgrades" sheetId="2" r:id="rId3"/>
+    <sheet name="Race Time Calculation" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drivers!$B$2:$I$24</definedName>
@@ -1540,8 +1540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,27 +1587,27 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D3" s="5">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="E3" s="4">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F3" s="4">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G3" s="4">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" ref="H3:H24" si="0">ROUND(AVERAGE(E3:G3),1)</f>
-        <v>96</v>
+        <f>ROUND(AVERAGE(E3:G3),1)</f>
+        <v>84</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I24" si="1">(ROUND((H3/1.5)*1200000*1.1,-5))/1000000</f>
-        <v>84.5</v>
+        <f>(ROUND((H3/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>73.900000000000006</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -1615,27 +1615,27 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D4" s="5">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="E4" s="4">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="F4" s="4">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="G4" s="4">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" si="0"/>
-        <v>95</v>
+        <f>ROUND(AVERAGE(E4:G4),1)</f>
+        <v>82.3</v>
       </c>
       <c r="I4" s="4">
-        <f t="shared" si="1"/>
-        <v>83.6</v>
+        <f>(ROUND((H4/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>72.400000000000006</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -1643,27 +1643,27 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D5" s="5">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F5" s="4">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="G5" s="4">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="0"/>
-        <v>94.7</v>
+        <f>ROUND(AVERAGE(E5:G5),1)</f>
+        <v>77.3</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" si="1"/>
-        <v>83.3</v>
+        <f>(ROUND((H5/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -1671,27 +1671,27 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D6" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E6" s="4">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="F6" s="4">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="G6" s="4">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="0"/>
-        <v>94</v>
+        <f>ROUND(AVERAGE(E6:G6),1)</f>
+        <v>75</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="1"/>
-        <v>82.7</v>
+        <f>(ROUND((H6/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
@@ -1699,55 +1699,55 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E7" s="4">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F7" s="4">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="G7" s="4">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="0"/>
-        <v>92.3</v>
+        <f>ROUND(AVERAGE(E7:G7),1)</f>
+        <v>76.7</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="1"/>
-        <v>81.2</v>
+        <f>(ROUND((H7/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>67.5</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="66">
+      <c r="B8" s="67">
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D8" s="5">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E8" s="4">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="F8" s="4">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="G8" s="4">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="0"/>
-        <v>90.7</v>
+        <f>ROUND(AVERAGE(E8:G8),1)</f>
+        <v>70</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="1"/>
-        <v>79.8</v>
+        <f>(ROUND((H8/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>61.6</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -1755,27 +1755,27 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>160</v>
+        <v>1</v>
       </c>
       <c r="D9" s="5">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="E9" s="4">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F9" s="4">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="G9" s="4">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="0"/>
-        <v>85.7</v>
+        <f>ROUND(AVERAGE(E9:G9),1)</f>
+        <v>94.7</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="1"/>
-        <v>75.400000000000006</v>
+        <f>(ROUND((H9/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>83.3</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
@@ -1783,27 +1783,27 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>159</v>
       </c>
       <c r="D10" s="5">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E10" s="4">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F10" s="4">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="G10" s="4">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="0"/>
-        <v>84</v>
+        <f>ROUND(AVERAGE(E10:G10),1)</f>
+        <v>71</v>
       </c>
       <c r="I10" s="4">
-        <f t="shared" si="1"/>
-        <v>73.900000000000006</v>
+        <f>(ROUND((H10/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>62.5</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -1811,27 +1811,27 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D11" s="5">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="E11" s="4">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F11" s="4">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G11" s="4">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="0"/>
-        <v>82.3</v>
+        <f>ROUND(AVERAGE(E11:G11),1)</f>
+        <v>79.7</v>
       </c>
       <c r="I11" s="4">
-        <f t="shared" si="1"/>
-        <v>72.400000000000006</v>
+        <f>(ROUND((H11/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>70.099999999999994</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
@@ -1839,27 +1839,27 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D12" s="5">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="4">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F12" s="4">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G12" s="4">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="0"/>
-        <v>79.7</v>
+        <f>ROUND(AVERAGE(E12:G12),1)</f>
+        <v>74</v>
       </c>
       <c r="I12" s="4">
-        <f t="shared" si="1"/>
-        <v>70.099999999999994</v>
+        <f>(ROUND((H12/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>65.099999999999994</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -1867,27 +1867,27 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D13" s="5">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="E13" s="4">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F13" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G13" s="4">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="0"/>
-        <v>79</v>
+        <f>ROUND(AVERAGE(E13:G13),1)</f>
+        <v>78.7</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="1"/>
-        <v>69.5</v>
+        <f>(ROUND((H13/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>69.3</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
@@ -1895,27 +1895,27 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D14" s="5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="4">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F14" s="4">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G14" s="4">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="0"/>
-        <v>78.7</v>
+        <f>ROUND(AVERAGE(E14:G14),1)</f>
+        <v>77.7</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="1"/>
-        <v>69.3</v>
+        <f>(ROUND((H14/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>68.400000000000006</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -1923,27 +1923,27 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D15" s="5">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E15" s="4">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F15" s="4">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G15" s="4">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="0"/>
-        <v>77.7</v>
+        <f>ROUND(AVERAGE(E15:G15),1)</f>
+        <v>77</v>
       </c>
       <c r="I15" s="4">
-        <f t="shared" si="1"/>
-        <v>68.400000000000006</v>
+        <f>(ROUND((H15/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>67.8</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
@@ -1951,27 +1951,27 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D16" s="5">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="E16" s="4">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F16" s="4">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G16" s="4">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="0"/>
-        <v>77.3</v>
+        <f>ROUND(AVERAGE(E16:G16),1)</f>
+        <v>72</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="1"/>
-        <v>68</v>
+        <f>(ROUND((H16/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>63.4</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -1979,27 +1979,27 @@
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>160</v>
       </c>
       <c r="D17" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="4">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="F17" s="4">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G17" s="4">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="0"/>
-        <v>77</v>
+        <f>ROUND(AVERAGE(E17:G17),1)</f>
+        <v>85.7</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="1"/>
-        <v>67.8</v>
+        <f>(ROUND((H17/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>75.400000000000006</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -2007,27 +2007,27 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D18" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18" s="4">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="F18" s="4">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="G18" s="4">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="0"/>
-        <v>76.7</v>
+        <f>ROUND(AVERAGE(E18:G18),1)</f>
+        <v>90.7</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="1"/>
-        <v>67.5</v>
+        <f>(ROUND((H18/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>79.8</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -2035,27 +2035,27 @@
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D19" s="5">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4">
+        <v>93</v>
+      </c>
+      <c r="F19" s="4">
         <v>94</v>
       </c>
-      <c r="E19" s="4">
-        <v>74</v>
-      </c>
-      <c r="F19" s="4">
-        <v>78</v>
-      </c>
       <c r="G19" s="4">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="0"/>
-        <v>75.3</v>
+        <f>ROUND(AVERAGE(E19:G19),1)</f>
+        <v>92.3</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="1"/>
-        <v>66.3</v>
+        <f>(ROUND((H19/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>81.2</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -2063,27 +2063,27 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D20" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E20" s="4">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="F20" s="4">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="G20" s="4">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="0"/>
-        <v>75</v>
+        <f>ROUND(AVERAGE(E20:G20),1)</f>
+        <v>95</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="1"/>
-        <v>66</v>
+        <f>(ROUND((H20/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>83.6</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -2091,27 +2091,27 @@
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D21" s="5">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="E21" s="4">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F21" s="4">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G21" s="4">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="0"/>
-        <v>74</v>
+        <f>ROUND(AVERAGE(E21:G21),1)</f>
+        <v>79</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="1"/>
-        <v>65.099999999999994</v>
+        <f>(ROUND((H21/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>69.5</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -2119,27 +2119,27 @@
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D22" s="5">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E22" s="4">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="F22" s="4">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="G22" s="4">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="0"/>
-        <v>72</v>
+        <f>ROUND(AVERAGE(E22:G22),1)</f>
+        <v>96</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="1"/>
-        <v>63.4</v>
+        <f>(ROUND((H22/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>84.5</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -2147,55 +2147,55 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>159</v>
+        <v>3</v>
       </c>
       <c r="D23" s="5">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="E23" s="4">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="F23" s="4">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="G23" s="4">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="0"/>
-        <v>71</v>
+        <f>ROUND(AVERAGE(E23:G23),1)</f>
+        <v>94</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="1"/>
-        <v>62.5</v>
+        <f>(ROUND((H23/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>82.7</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="67">
+      <c r="B24" s="66">
         <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D24" s="5">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="E24" s="4">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F24" s="4">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="G24" s="4">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="0"/>
-        <v>70</v>
+        <f>ROUND(AVERAGE(E24:G24),1)</f>
+        <v>75.3</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="1"/>
-        <v>61.6</v>
+        <f>(ROUND((H24/1.5)*1200000*1.1,-5))/1000000</f>
+        <v>66.3</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -2282,6 +2282,306 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F24"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="70" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="70" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="68">
+        <v>1</v>
+      </c>
+      <c r="C3" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="66">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="68">
+        <v>2</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="66">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="68">
+        <v>3</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="66">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="68">
+        <v>4</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="66">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="68">
+        <v>5</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="66">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="68">
+        <v>6</v>
+      </c>
+      <c r="C8" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="66">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="68">
+        <v>7</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="66">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="68">
+        <v>8</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="66">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="68">
+        <v>9</v>
+      </c>
+      <c r="C11" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="66">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="68">
+        <v>10</v>
+      </c>
+      <c r="C12" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="66">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="68">
+        <v>11</v>
+      </c>
+      <c r="C13" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="66">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="68">
+        <v>12</v>
+      </c>
+      <c r="C14" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="68"/>
+      <c r="F14" s="53"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="68">
+        <v>13</v>
+      </c>
+      <c r="C15" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="68"/>
+      <c r="F15" s="53"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="68">
+        <v>14</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="68"/>
+      <c r="F16" s="53"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="68">
+        <v>15</v>
+      </c>
+      <c r="C17" s="73" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="68"/>
+      <c r="F17" s="53"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="68">
+        <v>16</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="68"/>
+      <c r="F18" s="53"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="68">
+        <v>17</v>
+      </c>
+      <c r="C19" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="68"/>
+      <c r="F19" s="53"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="68">
+        <v>18</v>
+      </c>
+      <c r="C20" s="73" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="68"/>
+      <c r="F20" s="53"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="68">
+        <v>19</v>
+      </c>
+      <c r="C21" s="73" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="68"/>
+      <c r="F21" s="53"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="68">
+        <v>20</v>
+      </c>
+      <c r="C22" s="73" t="s">
+        <v>198</v>
+      </c>
+      <c r="E22" s="68"/>
+      <c r="F22" s="53"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="68">
+        <v>21</v>
+      </c>
+      <c r="C23" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="68"/>
+      <c r="F23" s="53"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="69">
+        <v>22</v>
+      </c>
+      <c r="C24" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="69"/>
+      <c r="F24" s="53"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K37"/>
   <sheetViews>
@@ -3094,7 +3394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
@@ -3870,304 +4170,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="s">
-        <v>185</v>
-      </c>
-      <c r="C2" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="70" t="s">
-        <v>186</v>
-      </c>
-      <c r="F2" s="72" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="68">
-        <v>1</v>
-      </c>
-      <c r="C3" s="74" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="66">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="68">
-        <v>2</v>
-      </c>
-      <c r="C4" s="73" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="66">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="68">
-        <v>3</v>
-      </c>
-      <c r="C5" s="73" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="66">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="68">
-        <v>4</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="66">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="68">
-        <v>5</v>
-      </c>
-      <c r="C7" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="66">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="68">
-        <v>6</v>
-      </c>
-      <c r="C8" s="73" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="66">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="68">
-        <v>7</v>
-      </c>
-      <c r="C9" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="66">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="68">
-        <v>8</v>
-      </c>
-      <c r="C10" s="73" t="s">
-        <v>159</v>
-      </c>
-      <c r="E10" s="66">
-        <v>8</v>
-      </c>
-      <c r="F10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="68">
-        <v>9</v>
-      </c>
-      <c r="C11" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="66">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="68">
-        <v>10</v>
-      </c>
-      <c r="C12" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="66">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="68">
-        <v>11</v>
-      </c>
-      <c r="C13" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="66">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="68">
-        <v>12</v>
-      </c>
-      <c r="C14" s="73" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="68"/>
-      <c r="F14" s="53"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="68">
-        <v>13</v>
-      </c>
-      <c r="C15" s="73" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="68"/>
-      <c r="F15" s="53"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="68">
-        <v>14</v>
-      </c>
-      <c r="C16" s="73" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="68"/>
-      <c r="F16" s="53"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="68">
-        <v>15</v>
-      </c>
-      <c r="C17" s="73" t="s">
-        <v>160</v>
-      </c>
-      <c r="E17" s="68"/>
-      <c r="F17" s="53"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="68">
-        <v>16</v>
-      </c>
-      <c r="C18" s="73" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="68"/>
-      <c r="F18" s="53"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="68">
-        <v>17</v>
-      </c>
-      <c r="C19" s="73" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="68"/>
-      <c r="F19" s="53"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="68">
-        <v>18</v>
-      </c>
-      <c r="C20" s="73" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="68"/>
-      <c r="F20" s="53"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="68">
-        <v>19</v>
-      </c>
-      <c r="C21" s="73" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="68"/>
-      <c r="F21" s="53"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="68">
-        <v>20</v>
-      </c>
-      <c r="C22" s="73" t="s">
-        <v>198</v>
-      </c>
-      <c r="E22" s="68"/>
-      <c r="F22" s="53"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="68">
-        <v>21</v>
-      </c>
-      <c r="C23" s="73" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="68"/>
-      <c r="F23" s="53"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="69">
-        <v>22</v>
-      </c>
-      <c r="C24" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="69"/>
-      <c r="F24" s="53"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
All drivers will now be created in the right car, looking at the team of the driver. Updated ID's in game data excel.
</commit_message>
<xml_diff>
--- a/Docs/GameData.xlsx
+++ b/Docs/GameData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Drivers" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Drivers!$B$2:$I$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ID''s'!$B$2:$E$24</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="200">
   <si>
     <t>Name</t>
   </si>
@@ -600,9 +601,6 @@
     <t>Manor</t>
   </si>
   <si>
-    <t>McLaren</t>
-  </si>
-  <si>
     <t>Mercedes</t>
   </si>
   <si>
@@ -622,6 +620,12 @@
   </si>
   <si>
     <t xml:space="preserve">Max Verstappen  </t>
+  </si>
+  <si>
+    <t>McLaren Honda</t>
+  </si>
+  <si>
+    <t>Team Name</t>
   </si>
 </sst>
 </file>
@@ -679,7 +683,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -997,17 +1001,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1198,8 +1191,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1540,7 +1533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1602,11 +1595,11 @@
         <v>82</v>
       </c>
       <c r="H3" s="4">
-        <f>ROUND(AVERAGE(E3:G3),1)</f>
+        <f t="shared" ref="H3:H24" si="0">ROUND(AVERAGE(E3:G3),1)</f>
         <v>84</v>
       </c>
       <c r="I3" s="4">
-        <f>(ROUND((H3/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" ref="I3:I24" si="1">(ROUND((H3/1.5)*1200000*1.1,-5))/1000000</f>
         <v>73.900000000000006</v>
       </c>
     </row>
@@ -1630,11 +1623,11 @@
         <v>83</v>
       </c>
       <c r="H4" s="4">
-        <f>ROUND(AVERAGE(E4:G4),1)</f>
+        <f t="shared" si="0"/>
         <v>82.3</v>
       </c>
       <c r="I4" s="4">
-        <f>(ROUND((H4/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>72.400000000000006</v>
       </c>
     </row>
@@ -1658,11 +1651,11 @@
         <v>80</v>
       </c>
       <c r="H5" s="4">
-        <f>ROUND(AVERAGE(E5:G5),1)</f>
+        <f t="shared" si="0"/>
         <v>77.3</v>
       </c>
       <c r="I5" s="4">
-        <f>(ROUND((H5/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>68</v>
       </c>
     </row>
@@ -1686,11 +1679,11 @@
         <v>71</v>
       </c>
       <c r="H6" s="4">
-        <f>ROUND(AVERAGE(E6:G6),1)</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
       <c r="I6" s="4">
-        <f>(ROUND((H6/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
     </row>
@@ -1714,11 +1707,11 @@
         <v>75</v>
       </c>
       <c r="H7" s="4">
-        <f>ROUND(AVERAGE(E7:G7),1)</f>
+        <f t="shared" si="0"/>
         <v>76.7</v>
       </c>
       <c r="I7" s="4">
-        <f>(ROUND((H7/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>67.5</v>
       </c>
     </row>
@@ -1742,11 +1735,11 @@
         <v>69</v>
       </c>
       <c r="H8" s="4">
-        <f>ROUND(AVERAGE(E8:G8),1)</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="I8" s="4">
-        <f>(ROUND((H8/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>61.6</v>
       </c>
     </row>
@@ -1770,11 +1763,11 @@
         <v>95</v>
       </c>
       <c r="H9" s="4">
-        <f>ROUND(AVERAGE(E9:G9),1)</f>
+        <f t="shared" si="0"/>
         <v>94.7</v>
       </c>
       <c r="I9" s="4">
-        <f>(ROUND((H9/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>83.3</v>
       </c>
     </row>
@@ -1798,11 +1791,11 @@
         <v>72</v>
       </c>
       <c r="H10" s="4">
-        <f>ROUND(AVERAGE(E10:G10),1)</f>
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="I10" s="4">
-        <f>(ROUND((H10/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>62.5</v>
       </c>
     </row>
@@ -1826,11 +1819,11 @@
         <v>82</v>
       </c>
       <c r="H11" s="4">
-        <f>ROUND(AVERAGE(E11:G11),1)</f>
+        <f t="shared" si="0"/>
         <v>79.7</v>
       </c>
       <c r="I11" s="4">
-        <f>(ROUND((H11/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>70.099999999999994</v>
       </c>
     </row>
@@ -1854,11 +1847,11 @@
         <v>74</v>
       </c>
       <c r="H12" s="4">
-        <f>ROUND(AVERAGE(E12:G12),1)</f>
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="I12" s="4">
-        <f>(ROUND((H12/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>65.099999999999994</v>
       </c>
     </row>
@@ -1882,11 +1875,11 @@
         <v>78</v>
       </c>
       <c r="H13" s="4">
-        <f>ROUND(AVERAGE(E13:G13),1)</f>
+        <f t="shared" si="0"/>
         <v>78.7</v>
       </c>
       <c r="I13" s="4">
-        <f>(ROUND((H13/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>69.3</v>
       </c>
     </row>
@@ -1910,11 +1903,11 @@
         <v>75</v>
       </c>
       <c r="H14" s="4">
-        <f>ROUND(AVERAGE(E14:G14),1)</f>
+        <f t="shared" si="0"/>
         <v>77.7</v>
       </c>
       <c r="I14" s="4">
-        <f>(ROUND((H14/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>68.400000000000006</v>
       </c>
     </row>
@@ -1938,11 +1931,11 @@
         <v>79</v>
       </c>
       <c r="H15" s="4">
-        <f>ROUND(AVERAGE(E15:G15),1)</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="I15" s="4">
-        <f>(ROUND((H15/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>67.8</v>
       </c>
     </row>
@@ -1966,11 +1959,11 @@
         <v>71</v>
       </c>
       <c r="H16" s="4">
-        <f>ROUND(AVERAGE(E16:G16),1)</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="I16" s="4">
-        <f>(ROUND((H16/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>63.4</v>
       </c>
     </row>
@@ -1994,11 +1987,11 @@
         <v>85</v>
       </c>
       <c r="H17" s="4">
-        <f>ROUND(AVERAGE(E17:G17),1)</f>
+        <f t="shared" si="0"/>
         <v>85.7</v>
       </c>
       <c r="I17" s="4">
-        <f>(ROUND((H17/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>75.400000000000006</v>
       </c>
     </row>
@@ -2022,11 +2015,11 @@
         <v>90</v>
       </c>
       <c r="H18" s="4">
-        <f>ROUND(AVERAGE(E18:G18),1)</f>
+        <f t="shared" si="0"/>
         <v>90.7</v>
       </c>
       <c r="I18" s="4">
-        <f>(ROUND((H18/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>79.8</v>
       </c>
     </row>
@@ -2050,11 +2043,11 @@
         <v>90</v>
       </c>
       <c r="H19" s="4">
-        <f>ROUND(AVERAGE(E19:G19),1)</f>
+        <f t="shared" si="0"/>
         <v>92.3</v>
       </c>
       <c r="I19" s="4">
-        <f>(ROUND((H19/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>81.2</v>
       </c>
     </row>
@@ -2078,11 +2071,11 @@
         <v>93</v>
       </c>
       <c r="H20" s="4">
-        <f>ROUND(AVERAGE(E20:G20),1)</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="I20" s="4">
-        <f>(ROUND((H20/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>83.6</v>
       </c>
     </row>
@@ -2106,11 +2099,11 @@
         <v>82</v>
       </c>
       <c r="H21" s="4">
-        <f>ROUND(AVERAGE(E21:G21),1)</f>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
       <c r="I21" s="4">
-        <f>(ROUND((H21/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>69.5</v>
       </c>
     </row>
@@ -2134,11 +2127,11 @@
         <v>96</v>
       </c>
       <c r="H22" s="4">
-        <f>ROUND(AVERAGE(E22:G22),1)</f>
+        <f t="shared" si="0"/>
         <v>96</v>
       </c>
       <c r="I22" s="4">
-        <f>(ROUND((H22/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>84.5</v>
       </c>
     </row>
@@ -2162,11 +2155,11 @@
         <v>94</v>
       </c>
       <c r="H23" s="4">
-        <f>ROUND(AVERAGE(E23:G23),1)</f>
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="I23" s="4">
-        <f>(ROUND((H23/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>82.7</v>
       </c>
     </row>
@@ -2190,11 +2183,11 @@
         <v>74</v>
       </c>
       <c r="H24" s="4">
-        <f>ROUND(AVERAGE(E24:G24),1)</f>
+        <f t="shared" si="0"/>
         <v>75.3</v>
       </c>
       <c r="I24" s="4">
-        <f>(ROUND((H24/1.5)*1200000*1.1,-5))/1000000</f>
+        <f t="shared" si="1"/>
         <v>66.3</v>
       </c>
     </row>
@@ -2283,10 +2276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F24"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,289 +2287,437 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="70" t="s">
         <v>185</v>
       </c>
       <c r="C2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="70" t="s">
+      <c r="D2" s="72" t="s">
         <v>186</v>
       </c>
-      <c r="F2" s="72" t="s">
+      <c r="E2" s="74" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" s="70" t="s">
+        <v>186</v>
+      </c>
+      <c r="H2" s="72" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="68">
         <v>1</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="66">
+      <c r="D3" s="68">
+        <v>5</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" s="66">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="68">
         <v>2</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="66">
+      <c r="D4" s="68">
+        <v>11</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" s="66">
         <v>2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="68">
         <v>3</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="66">
+      <c r="D5" s="68">
+        <v>5</v>
+      </c>
+      <c r="E5" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" s="66">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="68">
         <v>4</v>
       </c>
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="66">
+      <c r="D6" s="68">
+        <v>9</v>
+      </c>
+      <c r="E6" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="G6" s="66">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="68">
         <v>5</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="66">
+      <c r="D7" s="68">
+        <v>3</v>
+      </c>
+      <c r="E7" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7" s="66">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="68">
         <v>6</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="66">
+      <c r="D8" s="68">
+        <v>3</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="G8" s="66">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="68">
         <v>7</v>
       </c>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="66">
+      <c r="D9" s="68">
+        <v>6</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" s="66">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="68">
         <v>8</v>
       </c>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="E10" s="66">
+      <c r="D10" s="68">
+        <v>4</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="G10" s="66">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="68">
         <v>9</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="66">
+      <c r="D11" s="68">
+        <v>2</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="G11" s="66">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="68">
         <v>10</v>
       </c>
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="66">
+      <c r="D12" s="68">
         <v>10</v>
       </c>
-      <c r="F12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="G12" s="66">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="68">
         <v>11</v>
       </c>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="66">
+      <c r="D13" s="68">
+        <v>8</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>193</v>
+      </c>
+      <c r="G13" s="66">
         <v>11</v>
       </c>
-      <c r="F13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="68">
         <v>12</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="68"/>
-      <c r="F14" s="53"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="68">
+        <v>11</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="G14" s="68"/>
+      <c r="H14" s="53"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="68">
         <v>13</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="68"/>
-      <c r="F15" s="53"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="68">
+        <v>9</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="G15" s="68"/>
+      <c r="H15" s="53"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="68">
         <v>14</v>
       </c>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="68"/>
-      <c r="F16" s="53"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="68">
+        <v>8</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>193</v>
+      </c>
+      <c r="G16" s="68"/>
+      <c r="H16" s="53"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="68">
         <v>15</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="E17" s="68"/>
-      <c r="F17" s="53"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="68">
+        <v>2</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>188</v>
+      </c>
+      <c r="G17" s="68"/>
+      <c r="H17" s="53"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="68">
         <v>16</v>
       </c>
-      <c r="C18" s="73" t="s">
+      <c r="C18" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="68"/>
-      <c r="F18" s="53"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="68">
+        <v>1</v>
+      </c>
+      <c r="E18" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="G18" s="68"/>
+      <c r="H18" s="53"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="68">
         <v>17</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="68"/>
-      <c r="F19" s="53"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="68">
+        <v>7</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="G19" s="68"/>
+      <c r="H19" s="53"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="68">
         <v>18</v>
       </c>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="68"/>
-      <c r="F20" s="53"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="68">
+        <v>6</v>
+      </c>
+      <c r="E20" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="G20" s="68"/>
+      <c r="H20" s="53"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="68">
         <v>19</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="68"/>
-      <c r="F21" s="53"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="68">
+        <v>10</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="G21" s="68"/>
+      <c r="H21" s="53"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="68">
         <v>20</v>
       </c>
-      <c r="C22" s="73" t="s">
-        <v>198</v>
-      </c>
-      <c r="E22" s="68"/>
-      <c r="F22" s="53"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D22" s="68">
+        <v>7</v>
+      </c>
+      <c r="E22" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="G22" s="68"/>
+      <c r="H22" s="53"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="68">
         <v>21</v>
       </c>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="68"/>
-      <c r="F23" s="53"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="68">
+        <v>1</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="G23" s="68"/>
+      <c r="H23" s="53"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="69">
         <v>22</v>
       </c>
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="69"/>
-      <c r="F24" s="53"/>
+      <c r="D24" s="68">
+        <v>4</v>
+      </c>
+      <c r="E24" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="G24" s="69"/>
+      <c r="H24" s="53"/>
     </row>
   </sheetData>
+  <autoFilter ref="B2:E24">
+    <sortState ref="B3:E24">
+      <sortCondition ref="B2:B24"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="B3:D24">
+    <sortCondition ref="B2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>